<commit_message>
GDE-6729 Update EVG_CBAUAT04.xlsx and Facility_Notebook.robot
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="6" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UAT04_Runbook" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1" calcOnSave="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -57,13 +57,6 @@
     <font>
       <name val="Arial"/>
       <family val="2"/>
-      <color indexed="12"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
@@ -73,8 +66,15 @@
       <sz val="10"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <color theme="10"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -93,8 +93,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -126,11 +132,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -145,29 +165,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -178,13 +195,19 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -491,11 +514,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CX2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -506,79 +529,80 @@
     <col width="24" customWidth="1" style="1" min="4" max="4"/>
     <col width="28" customWidth="1" style="1" min="5" max="5"/>
     <col width="8.5703125" customWidth="1" style="1" min="6" max="6"/>
-    <col width="11.5703125" customWidth="1" style="1" min="7" max="7"/>
-    <col width="13.28515625" customWidth="1" style="1" min="8" max="8"/>
-    <col width="11.140625" customWidth="1" style="1" min="9" max="9"/>
-    <col width="57.7109375" customWidth="1" style="1" min="10" max="10"/>
-    <col width="15" customWidth="1" style="1" min="11" max="11"/>
-    <col width="19.140625" customWidth="1" style="1" min="12" max="12"/>
-    <col width="24.5703125" customWidth="1" style="1" min="13" max="13"/>
-    <col width="13.28515625" customWidth="1" style="1" min="14" max="14"/>
-    <col width="23" customWidth="1" style="1" min="15" max="15"/>
-    <col width="17" customWidth="1" style="1" min="16" max="16"/>
-    <col width="35" customWidth="1" style="1" min="17" max="17"/>
-    <col width="29" customWidth="1" style="1" min="18" max="18"/>
-    <col width="15.28515625" customWidth="1" style="1" min="19" max="19"/>
-    <col width="14.42578125" customWidth="1" style="1" min="20" max="20"/>
-    <col width="15.5703125" customWidth="1" style="1" min="21" max="21"/>
-    <col width="18.42578125" customWidth="1" style="1" min="22" max="22"/>
-    <col width="12" customWidth="1" style="1" min="23" max="23"/>
-    <col width="13.7109375" customWidth="1" style="1" min="24" max="24"/>
-    <col width="15.5703125" customWidth="1" style="1" min="25" max="25"/>
-    <col width="10.5703125" customWidth="1" style="1" min="26" max="26"/>
-    <col width="15.28515625" customWidth="1" style="1" min="27" max="28"/>
-    <col width="10.42578125" customWidth="1" style="1" min="29" max="29"/>
-    <col width="14.85546875" customWidth="1" style="1" min="30" max="30"/>
-    <col width="19.7109375" customWidth="1" style="1" min="31" max="31"/>
-    <col width="14" customWidth="1" style="1" min="32" max="32"/>
-    <col width="14.42578125" customWidth="1" style="1" min="33" max="33"/>
-    <col width="20.7109375" customWidth="1" style="1" min="34" max="34"/>
-    <col width="13.85546875" customWidth="1" style="1" min="35" max="35"/>
-    <col width="10" customWidth="1" style="1" min="36" max="36"/>
-    <col width="27.42578125" customWidth="1" style="1" min="37" max="37"/>
-    <col width="21.140625" customWidth="1" style="1" min="38" max="38"/>
-    <col width="24.28515625" customWidth="1" style="1" min="39" max="39"/>
-    <col width="18.42578125" customWidth="1" style="1" min="40" max="40"/>
-    <col width="28.85546875" customWidth="1" style="1" min="41" max="41"/>
-    <col width="14.28515625" customWidth="1" style="1" min="42" max="42"/>
-    <col width="23" customWidth="1" style="1" min="43" max="43"/>
-    <col width="19.85546875" customWidth="1" style="1" min="44" max="47"/>
-    <col width="24.7109375" customWidth="1" style="1" min="48" max="49"/>
-    <col width="25" customWidth="1" style="1" min="50" max="50"/>
-    <col width="24.42578125" customWidth="1" style="1" min="51" max="51"/>
-    <col width="30.42578125" customWidth="1" style="1" min="52" max="52"/>
-    <col width="36" customWidth="1" style="1" min="53" max="53"/>
-    <col width="34.42578125" customWidth="1" style="1" min="54" max="54"/>
-    <col width="26.7109375" customWidth="1" style="1" min="55" max="55"/>
-    <col width="17.28515625" customWidth="1" style="1" min="56" max="57"/>
-    <col width="34.140625" customWidth="1" style="1" min="58" max="58"/>
-    <col width="28.42578125" customWidth="1" style="1" min="59" max="59"/>
-    <col width="24.7109375" customWidth="1" style="1" min="60" max="60"/>
-    <col width="30.28515625" customWidth="1" style="1" min="61" max="61"/>
-    <col width="17.5703125" customWidth="1" style="1" min="62" max="62"/>
-    <col width="20.28515625" customWidth="1" style="1" min="63" max="63"/>
-    <col width="12.140625" customWidth="1" style="1" min="64" max="64"/>
-    <col width="21.42578125" customWidth="1" style="1" min="65" max="65"/>
-    <col width="24.140625" customWidth="1" style="1" min="66" max="66"/>
-    <col width="16" customWidth="1" style="1" min="67" max="67"/>
-    <col width="14" customWidth="1" style="1" min="68" max="68"/>
-    <col width="16.7109375" customWidth="1" style="1" min="69" max="69"/>
-    <col width="10.42578125" customWidth="1" style="1" min="70" max="70"/>
-    <col width="37.7109375" customWidth="1" style="1" min="71" max="71"/>
-    <col width="16.7109375" customWidth="1" style="1" min="72" max="73"/>
-    <col width="20.140625" customWidth="1" style="1" min="74" max="76"/>
-    <col width="17.7109375" customWidth="1" style="1" min="77" max="77"/>
-    <col width="24.5703125" customWidth="1" style="1" min="78" max="78"/>
-    <col width="19.42578125" customWidth="1" style="1" min="79" max="81"/>
-    <col width="21.140625" customWidth="1" style="1" min="82" max="82"/>
-    <col width="32.42578125" customWidth="1" style="1" min="83" max="83"/>
-    <col width="17.28515625" customWidth="1" style="1" min="84" max="85"/>
-    <col width="17.5703125" customWidth="1" style="1" min="86" max="88"/>
-    <col width="26.28515625" customWidth="1" style="1" min="89" max="89"/>
-    <col width="35" customWidth="1" style="1" min="90" max="90"/>
-    <col width="26.5703125" customWidth="1" style="1" min="91" max="91"/>
-    <col width="24.85546875" customWidth="1" style="1" min="92" max="92"/>
-    <col width="20" customWidth="1" style="1" min="93" max="93"/>
+    <col width="28" bestFit="1" customWidth="1" style="1" min="7" max="7"/>
+    <col width="11.5703125" customWidth="1" style="1" min="8" max="8"/>
+    <col width="13.28515625" customWidth="1" style="1" min="9" max="9"/>
+    <col width="11.140625" customWidth="1" style="1" min="10" max="10"/>
+    <col width="57.7109375" customWidth="1" style="1" min="11" max="11"/>
+    <col width="15" customWidth="1" style="1" min="12" max="12"/>
+    <col width="19.140625" customWidth="1" style="1" min="13" max="13"/>
+    <col width="24.5703125" customWidth="1" style="1" min="14" max="14"/>
+    <col width="13.28515625" customWidth="1" style="1" min="15" max="15"/>
+    <col width="23" customWidth="1" style="1" min="16" max="16"/>
+    <col width="17" customWidth="1" style="1" min="17" max="17"/>
+    <col width="35" customWidth="1" style="1" min="18" max="18"/>
+    <col width="29" customWidth="1" style="1" min="19" max="19"/>
+    <col width="15.28515625" customWidth="1" style="1" min="20" max="20"/>
+    <col width="14.42578125" customWidth="1" style="1" min="21" max="21"/>
+    <col width="15.5703125" customWidth="1" style="1" min="22" max="22"/>
+    <col width="18.42578125" customWidth="1" style="1" min="23" max="23"/>
+    <col width="12" customWidth="1" style="1" min="24" max="24"/>
+    <col width="13.7109375" customWidth="1" style="1" min="25" max="25"/>
+    <col width="15.5703125" customWidth="1" style="1" min="26" max="26"/>
+    <col width="10.5703125" customWidth="1" style="1" min="27" max="27"/>
+    <col width="15.28515625" customWidth="1" style="1" min="28" max="29"/>
+    <col width="10.42578125" customWidth="1" style="1" min="30" max="30"/>
+    <col width="14.85546875" customWidth="1" style="1" min="31" max="31"/>
+    <col width="19.7109375" customWidth="1" style="1" min="32" max="32"/>
+    <col width="14" customWidth="1" style="1" min="33" max="33"/>
+    <col width="14.42578125" customWidth="1" style="1" min="34" max="34"/>
+    <col width="20.7109375" customWidth="1" style="1" min="35" max="35"/>
+    <col width="13.85546875" customWidth="1" style="1" min="36" max="36"/>
+    <col width="10" customWidth="1" style="1" min="37" max="37"/>
+    <col width="27.42578125" customWidth="1" style="1" min="38" max="38"/>
+    <col width="21.140625" customWidth="1" style="1" min="39" max="39"/>
+    <col width="24.28515625" customWidth="1" style="1" min="40" max="40"/>
+    <col width="18.42578125" customWidth="1" style="1" min="41" max="41"/>
+    <col width="28.85546875" customWidth="1" style="1" min="42" max="42"/>
+    <col width="14.28515625" customWidth="1" style="1" min="43" max="43"/>
+    <col width="23" customWidth="1" style="1" min="44" max="44"/>
+    <col width="19.85546875" customWidth="1" style="1" min="45" max="48"/>
+    <col width="24.7109375" customWidth="1" style="1" min="49" max="50"/>
+    <col width="25" customWidth="1" style="1" min="51" max="51"/>
+    <col width="24.42578125" customWidth="1" style="1" min="52" max="52"/>
+    <col width="30.42578125" customWidth="1" style="1" min="53" max="53"/>
+    <col width="36" customWidth="1" style="1" min="54" max="54"/>
+    <col width="34.42578125" customWidth="1" style="1" min="55" max="55"/>
+    <col width="26.7109375" customWidth="1" style="1" min="56" max="56"/>
+    <col width="17.28515625" customWidth="1" style="1" min="57" max="58"/>
+    <col width="34.140625" customWidth="1" style="1" min="59" max="59"/>
+    <col width="28.42578125" customWidth="1" style="1" min="60" max="60"/>
+    <col width="24.7109375" customWidth="1" style="1" min="61" max="61"/>
+    <col width="30.28515625" customWidth="1" style="1" min="62" max="62"/>
+    <col width="17.5703125" customWidth="1" style="1" min="63" max="63"/>
+    <col width="20.28515625" customWidth="1" style="1" min="64" max="64"/>
+    <col width="12.140625" customWidth="1" style="1" min="65" max="65"/>
+    <col width="21.42578125" customWidth="1" style="1" min="66" max="66"/>
+    <col width="24.140625" customWidth="1" style="1" min="67" max="67"/>
+    <col width="16" customWidth="1" style="1" min="68" max="68"/>
+    <col width="14" customWidth="1" style="1" min="69" max="69"/>
+    <col width="16.7109375" customWidth="1" style="1" min="70" max="70"/>
+    <col width="10.42578125" customWidth="1" style="1" min="71" max="71"/>
+    <col width="37.7109375" customWidth="1" style="1" min="72" max="72"/>
+    <col width="16.7109375" customWidth="1" style="1" min="73" max="74"/>
+    <col width="20.140625" customWidth="1" style="1" min="75" max="77"/>
+    <col width="17.7109375" customWidth="1" style="1" min="78" max="78"/>
+    <col width="24.5703125" customWidth="1" style="1" min="79" max="79"/>
+    <col width="19.42578125" customWidth="1" style="1" min="80" max="82"/>
+    <col width="21.140625" customWidth="1" style="1" min="83" max="83"/>
+    <col width="32.42578125" customWidth="1" style="1" min="84" max="84"/>
+    <col width="17.28515625" customWidth="1" style="1" min="85" max="86"/>
+    <col width="17.5703125" customWidth="1" style="1" min="87" max="89"/>
+    <col width="26.28515625" customWidth="1" style="1" min="90" max="90"/>
+    <col width="35" customWidth="1" style="1" min="91" max="91"/>
+    <col width="26.5703125" customWidth="1" style="1" min="92" max="92"/>
+    <col width="24.85546875" customWidth="1" style="1" min="93" max="93"/>
+    <col width="20" customWidth="1" style="1" min="94" max="94"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="2">
@@ -614,175 +638,179 @@
       </c>
       <c r="G1" s="4" t="inlineStr">
         <is>
+          <t>Short_Name</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
           <t>Locality</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Branch_Code</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>Party_Type</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>Party_Sub_Type</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>Party_Category</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>Registered_Number</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>Country_of_Tax_Domicile</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>Date_Formed</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>Country_of_Registration</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>Business_Country</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>Industry_Sector</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>Business_Activity</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>Business_Focus</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>Business_Type</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>Is_Main_Activity</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>Is_Primary_Activity</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>GSTID</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>Address_Type</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>Country_Region</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>Post_Code</t>
         </is>
       </c>
-      <c r="AA1" s="4" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>Address_Line_1</t>
         </is>
       </c>
-      <c r="AB1" s="4" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>Address_Line_2</t>
         </is>
       </c>
-      <c r="AC1" s="4" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>Town_City</t>
         </is>
       </c>
-      <c r="AD1" s="4" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>State_Province</t>
         </is>
       </c>
-      <c r="AE1" s="4" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>Email_Contact_Type</t>
         </is>
       </c>
-      <c r="AF1" s="4" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="AG1" s="4" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>Confirm_Email</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>Mobile_Contact_Type</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>Country_Code</t>
         </is>
       </c>
-      <c r="AJ1" s="4" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="AK1" s="4" t="inlineStr">
+      <c r="AL1" s="4" t="inlineStr">
         <is>
           <t>Document_Collection_Status</t>
         </is>
       </c>
-      <c r="AL1" s="4" t="inlineStr">
+      <c r="AM1" s="4" t="inlineStr">
         <is>
           <t>Selected_Module</t>
         </is>
       </c>
-      <c r="AM1" s="4" t="inlineStr">
+      <c r="AN1" s="4" t="inlineStr">
         <is>
           <t>Task_ID_from_Supervisor</t>
         </is>
       </c>
-      <c r="AN1" s="4" t="inlineStr">
+      <c r="AO1" s="4" t="inlineStr">
         <is>
           <t>Task_ID_from_User</t>
         </is>
       </c>
-      <c r="AO1" s="4" t="n"/>
       <c r="AP1" s="4" t="n"/>
       <c r="AQ1" s="4" t="n"/>
       <c r="AR1" s="4" t="n"/>
@@ -835,6 +863,7 @@
       <c r="CM1" s="4" t="n"/>
       <c r="CN1" s="4" t="n"/>
       <c r="CO1" s="4" t="n"/>
+      <c r="CP1" s="4" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -849,7 +878,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY1315057</t>
+          <t>ARIHANT TRADING COMPANY 1714417</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -864,221 +893,230 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
+          <t>1714417</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1714417</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr">
         <is>
           <t>Local Private</t>
         </is>
       </c>
-      <c r="H2" s="5" t="inlineStr">
+      <c r="I2" s="5" t="inlineStr">
         <is>
           <t>00000001</t>
         </is>
       </c>
-      <c r="I2" s="5" t="inlineStr">
+      <c r="J2" s="5" t="inlineStr">
         <is>
           <t>Enterprise</t>
         </is>
       </c>
-      <c r="J2" s="6" t="inlineStr">
+      <c r="K2" s="6" t="inlineStr">
         <is>
           <t>Unlisted Company, Foreign Private Company Registered with ASIC</t>
         </is>
       </c>
-      <c r="K2" s="5" t="inlineStr">
+      <c r="L2" s="5" t="inlineStr">
         <is>
           <t>Full</t>
         </is>
       </c>
-      <c r="L2" s="1" t="inlineStr">
+      <c r="M2" s="1" t="inlineStr">
         <is>
           <t>1014001</t>
         </is>
       </c>
-      <c r="M2" s="5" t="inlineStr">
+      <c r="N2" s="5" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="N2" s="7" t="inlineStr">
+      <c r="O2" s="7" t="inlineStr">
         <is>
           <t>2015-04-06</t>
         </is>
       </c>
-      <c r="O2" s="7" t="inlineStr">
+      <c r="P2" s="7" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="P2" s="7" t="inlineStr">
+      <c r="Q2" s="7" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="Q2" s="5" t="inlineStr">
+      <c r="R2" s="5" t="inlineStr">
         <is>
           <t>Government Administration and Defence</t>
         </is>
       </c>
-      <c r="R2" s="5" t="inlineStr">
+      <c r="S2" s="5" t="inlineStr">
         <is>
           <t>State Government Administration</t>
         </is>
       </c>
-      <c r="S2" s="5" t="inlineStr">
+      <c r="T2" s="5" t="inlineStr">
         <is>
           <t>Both</t>
         </is>
       </c>
-      <c r="T2" s="5" t="inlineStr">
+      <c r="U2" s="5" t="inlineStr">
         <is>
           <t>Affinity</t>
         </is>
       </c>
-      <c r="U2" s="5" t="inlineStr">
+      <c r="V2" s="5" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="V2" s="5" t="inlineStr">
+      <c r="W2" s="5" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="W2" s="5" t="inlineStr">
+      <c r="X2" s="5" t="inlineStr">
         <is>
           <t>10075843210</t>
         </is>
       </c>
-      <c r="X2" s="5" t="inlineStr">
+      <c r="Y2" s="5" t="inlineStr">
         <is>
           <t>Legal Address</t>
         </is>
       </c>
-      <c r="Y2" s="5" t="inlineStr">
+      <c r="Z2" s="5" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="Z2" s="8" t="inlineStr">
+      <c r="AA2" s="8" t="inlineStr">
         <is>
           <t>4061</t>
         </is>
       </c>
-      <c r="AA2" s="5" t="inlineStr">
+      <c r="AB2" s="5" t="inlineStr">
         <is>
           <t>George St.</t>
         </is>
       </c>
-      <c r="AB2" s="5" t="inlineStr">
+      <c r="AC2" s="5" t="inlineStr">
         <is>
           <t>Beverly Hills</t>
         </is>
       </c>
-      <c r="AC2" s="9" t="inlineStr">
+      <c r="AD2" s="9" t="inlineStr">
         <is>
           <t>Melbourne</t>
         </is>
       </c>
-      <c r="AD2" s="9" t="inlineStr">
+      <c r="AE2" s="9" t="inlineStr">
         <is>
           <t>Victoria</t>
         </is>
       </c>
-      <c r="AE2" s="9" t="inlineStr">
+      <c r="AF2" s="9" t="inlineStr">
         <is>
           <t>Work</t>
         </is>
       </c>
-      <c r="AF2" s="10" t="inlineStr">
-        <is>
-          <t>evrl3@test.com</t>
-        </is>
-      </c>
-      <c r="AG2" s="10" t="inlineStr">
-        <is>
-          <t>evrl3@test.com</t>
-        </is>
-      </c>
-      <c r="AH2" s="9" t="inlineStr">
+      <c r="AG2" s="31" t="inlineStr">
+        <is>
+          <t>vinnie.jones@lockstock.com</t>
+        </is>
+      </c>
+      <c r="AH2" s="31" t="inlineStr">
+        <is>
+          <t>vinnie.jones@lockstock.com</t>
+        </is>
+      </c>
+      <c r="AI2" s="9" t="inlineStr">
         <is>
           <t>Work</t>
         </is>
       </c>
-      <c r="AI2" s="9" t="inlineStr">
+      <c r="AJ2" s="9" t="inlineStr">
         <is>
           <t>+61</t>
         </is>
       </c>
-      <c r="AJ2" s="9" t="inlineStr">
-        <is>
-          <t>442345679</t>
-        </is>
-      </c>
-      <c r="AK2" s="5" t="inlineStr">
+      <c r="AK2" s="32" t="inlineStr">
+        <is>
+          <t>0298761234</t>
+        </is>
+      </c>
+      <c r="AL2" s="5" t="inlineStr">
         <is>
           <t>Documents not collected</t>
         </is>
       </c>
-      <c r="AL2" s="5" t="inlineStr">
+      <c r="AM2" s="5" t="inlineStr">
         <is>
           <t>Quick Party Onboarding</t>
         </is>
       </c>
-      <c r="AM2" s="1" t="inlineStr">
+      <c r="AN2" s="1" t="inlineStr">
         <is>
           <t>1164f57726c6GBld</t>
         </is>
       </c>
-      <c r="AN2" s="1" t="inlineStr">
+      <c r="AO2" s="1" t="inlineStr">
         <is>
           <t>1164f57780d0GBvY</t>
         </is>
       </c>
-      <c r="CP2" s="1" t="inlineStr">
+      <c r="CQ2" s="1" t="inlineStr">
         <is>
           <t>1612526</t>
         </is>
       </c>
-      <c r="CQ2" s="1" t="inlineStr">
+      <c r="CR2" s="1" t="inlineStr">
         <is>
           <t>1613642</t>
         </is>
       </c>
-      <c r="CR2" s="1" t="inlineStr">
+      <c r="CS2" s="1" t="inlineStr">
         <is>
           <t>1614117</t>
         </is>
       </c>
-      <c r="CS2" s="1" t="inlineStr">
+      <c r="CT2" s="1" t="inlineStr">
         <is>
           <t>1614428</t>
         </is>
       </c>
-      <c r="CT2" s="1" t="inlineStr">
+      <c r="CU2" s="1" t="inlineStr">
         <is>
           <t>1712619</t>
         </is>
       </c>
-      <c r="CU2" s="1" t="inlineStr">
+      <c r="CV2" s="1" t="inlineStr">
         <is>
           <t>1810326</t>
         </is>
       </c>
-      <c r="CV2" s="1" t="inlineStr">
+      <c r="CW2" s="1" t="inlineStr">
         <is>
           <t>1313745</t>
         </is>
       </c>
-      <c r="CW2" s="1" t="inlineStr">
+      <c r="CX2" s="1" t="inlineStr">
         <is>
           <t>1315059</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AG2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AH2" r:id="rId2"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" pageOrder="overThenDown" horizontalDpi="300" verticalDpi="300"/>
@@ -1093,76 +1131,76 @@
   </sheetPr>
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView topLeftCell="AE1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="6.140625" customWidth="1" style="12" min="1" max="1"/>
-    <col width="37.42578125" customWidth="1" style="12" min="2" max="2"/>
-    <col width="49.85546875" customWidth="1" style="12" min="3" max="3"/>
-    <col width="20.5703125" customWidth="1" style="12" min="4" max="4"/>
-    <col width="15.7109375" customWidth="1" style="12" min="5" max="5"/>
-    <col width="27.28515625" customWidth="1" style="12" min="6" max="6"/>
-    <col width="14.5703125" customWidth="1" style="12" min="7" max="7"/>
-    <col width="16.85546875" customWidth="1" style="12" min="8" max="8"/>
-    <col width="16.42578125" customWidth="1" style="12" min="9" max="9"/>
-    <col width="33.28515625" customWidth="1" style="12" min="10" max="10"/>
-    <col width="12.42578125" customWidth="1" style="12" min="11" max="11"/>
-    <col width="22" customWidth="1" style="12" min="12" max="12"/>
-    <col width="12.5703125" customWidth="1" style="12" min="13" max="13"/>
-    <col width="15.7109375" customWidth="1" style="12" min="14" max="14"/>
-    <col width="23.7109375" customWidth="1" style="12" min="15" max="15"/>
-    <col width="18.28515625" customWidth="1" style="12" min="16" max="16"/>
-    <col width="18.140625" customWidth="1" style="12" min="17" max="17"/>
-    <col width="23.140625" customWidth="1" style="12" min="18" max="18"/>
-    <col width="21" customWidth="1" style="12" min="19" max="19"/>
-    <col width="25.5703125" customWidth="1" style="12" min="20" max="20"/>
-    <col width="21.7109375" customWidth="1" style="12" min="21" max="21"/>
-    <col width="18.7109375" customWidth="1" style="12" min="22" max="22"/>
-    <col width="14.5703125" customWidth="1" style="12" min="23" max="23"/>
-    <col width="16.7109375" customWidth="1" style="12" min="24" max="24"/>
-    <col width="14.28515625" customWidth="1" style="12" min="25" max="26"/>
-    <col width="12.5703125" customWidth="1" style="12" min="27" max="27"/>
-    <col width="16.28515625" customWidth="1" style="12" min="28" max="28"/>
-    <col width="12.85546875" customWidth="1" style="12" min="29" max="29"/>
-    <col width="21.85546875" customWidth="1" style="12" min="30" max="30"/>
-    <col width="14" customWidth="1" style="12" min="31" max="31"/>
-    <col width="22.5703125" customWidth="1" style="12" min="32" max="32"/>
-    <col width="37.140625" customWidth="1" style="12" min="33" max="33"/>
-    <col width="28" customWidth="1" style="12" min="34" max="34"/>
-    <col width="19" customWidth="1" style="12" min="35" max="35"/>
-    <col width="56.28515625" customWidth="1" style="12" min="36" max="36"/>
-    <col width="36.7109375" customWidth="1" style="12" min="37" max="37"/>
-    <col width="18.5703125" customWidth="1" style="12" min="38" max="38"/>
-    <col width="22" customWidth="1" style="12" min="39" max="39"/>
-    <col width="36.7109375" customWidth="1" style="12" min="40" max="40"/>
-    <col width="20" customWidth="1" style="12" min="41" max="41"/>
-    <col width="10" customWidth="1" style="12" min="42" max="42"/>
-    <col width="27.140625" customWidth="1" style="12" min="43" max="43"/>
-    <col width="22.28515625" customWidth="1" style="12" min="44" max="44"/>
-    <col width="25.85546875" customWidth="1" style="12" min="45" max="45"/>
-    <col width="30.85546875" customWidth="1" style="12" min="46" max="46"/>
-    <col width="28.140625" customWidth="1" style="12" min="47" max="47"/>
-    <col width="40.5703125" customWidth="1" style="12" min="48" max="49"/>
-    <col width="23" customWidth="1" style="12" min="50" max="50"/>
-    <col width="22.28515625" customWidth="1" style="12" min="51" max="51"/>
-    <col width="30.85546875" customWidth="1" style="12" min="52" max="52"/>
-    <col width="30" customWidth="1" style="12" min="53" max="53"/>
-    <col width="27.28515625" customWidth="1" style="12" min="54" max="54"/>
-    <col width="22.42578125" customWidth="1" style="12" min="55" max="55"/>
-    <col width="20" customWidth="1" style="12" min="56" max="56"/>
-    <col width="53.7109375" customWidth="1" style="12" min="57" max="57"/>
-    <col width="21.42578125" customWidth="1" style="12" min="58" max="58"/>
-    <col width="34.5703125" customWidth="1" style="12" min="59" max="59"/>
-    <col width="17.28515625" customWidth="1" style="12" min="60" max="60"/>
-    <col width="22.28515625" customWidth="1" style="12" min="61" max="61"/>
-    <col width="12.5703125" customWidth="1" style="12" min="62" max="62"/>
-    <col width="27.140625" customWidth="1" style="12" min="63" max="63"/>
-    <col width="16.42578125" customWidth="1" style="12" min="64" max="64"/>
-    <col width="19.85546875" customWidth="1" style="12" min="65" max="66"/>
-    <col width="31.140625" customWidth="1" style="12" min="67" max="67"/>
+    <col width="6.140625" customWidth="1" style="11" min="1" max="1"/>
+    <col width="37.42578125" customWidth="1" style="11" min="2" max="2"/>
+    <col width="49.85546875" customWidth="1" style="11" min="3" max="3"/>
+    <col width="20.5703125" customWidth="1" style="11" min="4" max="4"/>
+    <col width="15.7109375" customWidth="1" style="11" min="5" max="5"/>
+    <col width="27.28515625" customWidth="1" style="11" min="6" max="6"/>
+    <col width="14.5703125" customWidth="1" style="11" min="7" max="7"/>
+    <col width="16.85546875" customWidth="1" style="11" min="8" max="8"/>
+    <col width="16.42578125" customWidth="1" style="11" min="9" max="9"/>
+    <col width="33.28515625" customWidth="1" style="11" min="10" max="10"/>
+    <col width="12.42578125" customWidth="1" style="11" min="11" max="11"/>
+    <col width="22" customWidth="1" style="11" min="12" max="12"/>
+    <col width="12.5703125" customWidth="1" style="11" min="13" max="13"/>
+    <col width="15.7109375" customWidth="1" style="11" min="14" max="14"/>
+    <col width="23.7109375" customWidth="1" style="11" min="15" max="15"/>
+    <col width="18.28515625" customWidth="1" style="11" min="16" max="16"/>
+    <col width="18.140625" customWidth="1" style="11" min="17" max="17"/>
+    <col width="23.140625" customWidth="1" style="11" min="18" max="18"/>
+    <col width="21" customWidth="1" style="11" min="19" max="19"/>
+    <col width="25.5703125" customWidth="1" style="11" min="20" max="20"/>
+    <col width="21.7109375" customWidth="1" style="11" min="21" max="21"/>
+    <col width="18.7109375" customWidth="1" style="11" min="22" max="22"/>
+    <col width="14.5703125" customWidth="1" style="11" min="23" max="23"/>
+    <col width="16.7109375" customWidth="1" style="11" min="24" max="24"/>
+    <col width="14.28515625" customWidth="1" style="11" min="25" max="26"/>
+    <col width="12.5703125" customWidth="1" style="11" min="27" max="27"/>
+    <col width="16.28515625" customWidth="1" style="11" min="28" max="28"/>
+    <col width="12.85546875" customWidth="1" style="11" min="29" max="29"/>
+    <col width="21.85546875" customWidth="1" style="11" min="30" max="30"/>
+    <col width="14" customWidth="1" style="11" min="31" max="31"/>
+    <col width="22.5703125" customWidth="1" style="11" min="32" max="32"/>
+    <col width="37.140625" customWidth="1" style="11" min="33" max="33"/>
+    <col width="28" customWidth="1" style="11" min="34" max="34"/>
+    <col width="19" customWidth="1" style="11" min="35" max="35"/>
+    <col width="56.28515625" customWidth="1" style="11" min="36" max="36"/>
+    <col width="36.7109375" customWidth="1" style="11" min="37" max="37"/>
+    <col width="18.5703125" customWidth="1" style="11" min="38" max="38"/>
+    <col width="22" customWidth="1" style="11" min="39" max="39"/>
+    <col width="36.7109375" customWidth="1" style="11" min="40" max="40"/>
+    <col width="20" customWidth="1" style="11" min="41" max="41"/>
+    <col width="10" customWidth="1" style="11" min="42" max="42"/>
+    <col width="27.140625" customWidth="1" style="11" min="43" max="43"/>
+    <col width="22.28515625" customWidth="1" style="11" min="44" max="44"/>
+    <col width="25.85546875" customWidth="1" style="11" min="45" max="45"/>
+    <col width="30.85546875" customWidth="1" style="11" min="46" max="46"/>
+    <col width="28.140625" customWidth="1" style="11" min="47" max="47"/>
+    <col width="40.5703125" customWidth="1" style="11" min="48" max="49"/>
+    <col width="23" customWidth="1" style="11" min="50" max="50"/>
+    <col width="22.28515625" customWidth="1" style="11" min="51" max="51"/>
+    <col width="30.85546875" customWidth="1" style="11" min="52" max="52"/>
+    <col width="30" customWidth="1" style="11" min="53" max="53"/>
+    <col width="27.28515625" customWidth="1" style="11" min="54" max="54"/>
+    <col width="22.42578125" customWidth="1" style="11" min="55" max="55"/>
+    <col width="20" customWidth="1" style="11" min="56" max="56"/>
+    <col width="53.7109375" customWidth="1" style="11" min="57" max="57"/>
+    <col width="21.42578125" customWidth="1" style="11" min="58" max="58"/>
+    <col width="34.5703125" customWidth="1" style="11" min="59" max="59"/>
+    <col width="17.28515625" customWidth="1" style="11" min="60" max="60"/>
+    <col width="22.28515625" customWidth="1" style="11" min="61" max="61"/>
+    <col width="12.5703125" customWidth="1" style="11" min="62" max="62"/>
+    <col width="27.140625" customWidth="1" style="11" min="63" max="63"/>
+    <col width="16.42578125" customWidth="1" style="11" min="64" max="64"/>
+    <col width="19.85546875" customWidth="1" style="11" min="65" max="66"/>
+    <col width="31.140625" customWidth="1" style="11" min="67" max="67"/>
     <col width="18.42578125" customWidth="1" style="1" min="68" max="68"/>
     <col width="16.5703125" customWidth="1" style="1" min="69" max="69"/>
     <col width="20.42578125" customWidth="1" style="1" min="70" max="70"/>
@@ -1171,7 +1209,7 @@
     <col width="18.42578125" customWidth="1" style="1" min="73" max="73"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="11">
+    <row r="1" customFormat="1" s="10">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>rowid</t>
@@ -1392,7 +1430,7 @@
           <t>Contact_PrimaryPhone</t>
         </is>
       </c>
-      <c r="AS1" s="13" t="inlineStr">
+      <c r="AS1" s="12" t="inlineStr">
         <is>
           <t>Contact_ProductSelected</t>
         </is>
@@ -1402,693 +1440,693 @@
           <t>Contact_BalanceTypeSelected</t>
         </is>
       </c>
-      <c r="AU1" s="14" t="inlineStr">
+      <c r="AU1" s="13" t="inlineStr">
         <is>
           <t>RemittanceInstruction_Method</t>
         </is>
       </c>
-      <c r="AV1" s="14" t="inlineStr">
+      <c r="AV1" s="13" t="inlineStr">
         <is>
           <t>RemittanceInstruction_Description</t>
         </is>
       </c>
-      <c r="AW1" s="14" t="inlineStr">
+      <c r="AW1" s="13" t="inlineStr">
         <is>
           <t>RemittanceInstruction_Currency</t>
         </is>
       </c>
-      <c r="AX1" s="14" t="inlineStr">
+      <c r="AX1" s="13" t="inlineStr">
         <is>
           <t>ProductSBLC_Checkbox</t>
         </is>
       </c>
-      <c r="AY1" s="14" t="inlineStr">
+      <c r="AY1" s="13" t="inlineStr">
         <is>
           <t>ProductLoan_Checkbox</t>
         </is>
       </c>
-      <c r="AZ1" s="14" t="inlineStr">
+      <c r="AZ1" s="13" t="inlineStr">
         <is>
           <t>BalanceType_Principal_Checkbox</t>
         </is>
       </c>
-      <c r="BA1" s="14" t="inlineStr">
+      <c r="BA1" s="13" t="inlineStr">
         <is>
           <t>BalanceType_Interest_Checkbox</t>
         </is>
       </c>
-      <c r="BB1" s="14" t="inlineStr">
+      <c r="BB1" s="13" t="inlineStr">
         <is>
           <t>BalanceType_Fees_Checkbox</t>
         </is>
       </c>
-      <c r="BC1" s="14" t="inlineStr">
+      <c r="BC1" s="13" t="inlineStr">
         <is>
           <t>RI_FromCust_Checkbox</t>
         </is>
       </c>
-      <c r="BD1" s="14" t="inlineStr">
+      <c r="BD1" s="13" t="inlineStr">
         <is>
           <t>RI_ToCust_Checkbox</t>
         </is>
       </c>
-      <c r="BE1" s="15" t="inlineStr">
+      <c r="BE1" s="14" t="inlineStr">
         <is>
           <t>NoticesSummary</t>
         </is>
       </c>
-      <c r="BF1" s="14" t="inlineStr">
+      <c r="BF1" s="13" t="inlineStr">
         <is>
           <t>RI_AutoDoIt_Checkbox</t>
         </is>
       </c>
-      <c r="BG1" s="14" t="inlineStr">
+      <c r="BG1" s="13" t="inlineStr">
         <is>
           <t>RI_SendersCorrespondent_Checkbox</t>
         </is>
       </c>
-      <c r="BH1" s="14" t="inlineStr">
+      <c r="BH1" s="13" t="inlineStr">
         <is>
           <t>IMT_MessageCode</t>
         </is>
       </c>
-      <c r="BI1" s="14" t="inlineStr">
+      <c r="BI1" s="13" t="inlineStr">
         <is>
           <t>Swift_Role</t>
         </is>
       </c>
-      <c r="BJ1" s="14" t="inlineStr">
+      <c r="BJ1" s="13" t="inlineStr">
         <is>
           <t>SwiftID</t>
         </is>
       </c>
-      <c r="BK1" s="14" t="inlineStr">
+      <c r="BK1" s="13" t="inlineStr">
         <is>
           <t>Swift_Description</t>
         </is>
       </c>
-      <c r="BL1" s="14" t="inlineStr">
+      <c r="BL1" s="13" t="inlineStr">
         <is>
           <t>ClearingType</t>
         </is>
       </c>
-      <c r="BM1" s="14" t="inlineStr">
+      <c r="BM1" s="13" t="inlineStr">
         <is>
           <t>ClearingNumber</t>
         </is>
       </c>
-      <c r="BN1" s="14" t="inlineStr">
+      <c r="BN1" s="13" t="inlineStr">
         <is>
           <t>AccountNumber</t>
         </is>
       </c>
-      <c r="BO1" s="14" t="inlineStr">
+      <c r="BO1" s="13" t="inlineStr">
         <is>
           <t>BOC_Level</t>
         </is>
       </c>
-      <c r="BP1" s="14" t="inlineStr">
+      <c r="BP1" s="13" t="inlineStr">
         <is>
           <t>Details_Of_Charges</t>
         </is>
       </c>
-      <c r="BQ1" s="14" t="inlineStr">
+      <c r="BQ1" s="13" t="inlineStr">
         <is>
           <t>DetailsOfPayment</t>
         </is>
       </c>
-      <c r="BR1" s="14" t="inlineStr">
+      <c r="BR1" s="13" t="inlineStr">
         <is>
           <t>SenderToReceiverInfo</t>
         </is>
       </c>
-      <c r="BS1" s="14" t="inlineStr">
+      <c r="BS1" s="13" t="inlineStr">
         <is>
           <t>OrderingCustomer</t>
         </is>
       </c>
-      <c r="BT1" s="14" t="inlineStr">
+      <c r="BT1" s="13" t="inlineStr">
         <is>
           <t>Usename</t>
         </is>
       </c>
-      <c r="BU1" s="14" t="inlineStr">
+      <c r="BU1" s="13" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="25.5" customFormat="1" customHeight="1" s="16">
-      <c r="A2" s="16" t="inlineStr">
+    <row r="2" ht="25.5" customFormat="1" customHeight="1" s="15">
+      <c r="A2" s="15" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="16" t="inlineStr">
+      <c r="B2" s="15" t="inlineStr">
         <is>
           <t>EVG_PTYLIQ07 Scenario7 Bilateral Facility - Termination of a Facility</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY1315057</t>
-        </is>
-      </c>
-      <c r="D2" s="16" t="inlineStr">
+          <t>ARIHANT TRADING COMPANY 1714417</t>
+        </is>
+      </c>
+      <c r="D2" s="15" t="inlineStr">
         <is>
           <t>Search by Customer ID</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
-        </is>
-      </c>
-      <c r="F2" s="17" t="inlineStr">
+          <t>1714417</t>
+        </is>
+      </c>
+      <c r="F2" s="16" t="inlineStr">
         <is>
           <t>Faxes/Emails Only</t>
         </is>
       </c>
-      <c r="G2" s="18" t="inlineStr">
+      <c r="G2" s="17" t="inlineStr">
         <is>
           <t>TM_SAF</t>
         </is>
       </c>
-      <c r="H2" s="18" t="inlineStr">
+      <c r="H2" s="17" t="inlineStr">
         <is>
           <t>GLB</t>
         </is>
       </c>
-      <c r="I2" s="18" t="inlineStr">
+      <c r="I2" s="17" t="inlineStr">
         <is>
           <t>8112</t>
         </is>
       </c>
-      <c r="J2" s="18" t="inlineStr">
+      <c r="J2" s="17" t="inlineStr">
         <is>
           <t>AU / State Government Administration</t>
         </is>
       </c>
-      <c r="K2" s="18" t="inlineStr">
+      <c r="K2" s="17" t="inlineStr">
         <is>
           <t>Borrower</t>
         </is>
       </c>
-      <c r="L2" s="18" t="inlineStr">
+      <c r="L2" s="17" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="M2" s="18" t="inlineStr">
+      <c r="M2" s="17" t="inlineStr">
         <is>
           <t>1917472</t>
         </is>
       </c>
-      <c r="N2" s="18" t="inlineStr">
+      <c r="N2" s="17" t="inlineStr">
         <is>
           <t>Work Fax</t>
         </is>
       </c>
-      <c r="O2" s="1" t="inlineStr">
-        <is>
-          <t>1315059</t>
-        </is>
-      </c>
-      <c r="P2" s="18" t="inlineStr">
+      <c r="O2" s="17" t="inlineStr">
+        <is>
+          <t>1714417</t>
+        </is>
+      </c>
+      <c r="P2" s="17" t="inlineStr">
         <is>
           <t>Vinnie</t>
         </is>
       </c>
-      <c r="Q2" s="18" t="inlineStr">
+      <c r="Q2" s="17" t="inlineStr">
         <is>
           <t>Jones</t>
         </is>
       </c>
-      <c r="R2" s="18" t="inlineStr">
+      <c r="R2" s="17" t="inlineStr">
         <is>
           <t>131100</t>
         </is>
       </c>
-      <c r="S2" s="18" t="inlineStr">
+      <c r="S2" s="17" t="inlineStr">
         <is>
           <t>Servicing</t>
         </is>
       </c>
-      <c r="T2" s="18" t="inlineStr">
+      <c r="T2" s="17" t="inlineStr">
         <is>
           <t>SERV</t>
         </is>
       </c>
-      <c r="U2" s="18" t="inlineStr">
+      <c r="U2" s="17" t="inlineStr">
         <is>
           <t>CBA Email with PDF Attachment</t>
         </is>
       </c>
-      <c r="V2" s="19" t="inlineStr">
+      <c r="V2" s="18" t="inlineStr">
         <is>
           <t>portz.prany@cba.com.au</t>
         </is>
       </c>
-      <c r="W2" s="18" t="inlineStr">
+      <c r="W2" s="17" t="inlineStr">
         <is>
           <t>Jones</t>
         </is>
       </c>
-      <c r="X2" s="18" t="inlineStr">
+      <c r="X2" s="17" t="inlineStr">
         <is>
           <t>LEGAL ADDRESS</t>
         </is>
       </c>
-      <c r="Y2" s="18" t="inlineStr">
+      <c r="Y2" s="17" t="inlineStr">
         <is>
           <t>George St.</t>
         </is>
       </c>
-      <c r="Z2" s="18" t="inlineStr">
+      <c r="Z2" s="17" t="inlineStr">
         <is>
           <t>Beverly Hills</t>
         </is>
       </c>
-      <c r="AA2" s="18" t="inlineStr">
+      <c r="AA2" s="17" t="inlineStr">
         <is>
           <t>Melbourne</t>
         </is>
       </c>
-      <c r="AB2" s="18" t="inlineStr">
+      <c r="AB2" s="17" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="AC2" s="18" t="inlineStr">
+      <c r="AC2" s="17" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="AD2" s="18" t="inlineStr">
+      <c r="AD2" s="17" t="inlineStr">
         <is>
           <t xml:space="preserve">412345678
  </t>
         </is>
       </c>
-      <c r="AE2" s="18" t="inlineStr">
+      <c r="AE2" s="17" t="inlineStr">
         <is>
           <t>Victoria</t>
         </is>
       </c>
-      <c r="AF2" s="18" t="inlineStr">
+      <c r="AF2" s="17" t="inlineStr">
         <is>
           <t>4061</t>
         </is>
       </c>
-      <c r="AG2" s="18" t="inlineStr">
+      <c r="AG2" s="17" t="inlineStr">
         <is>
           <t>CFS QLD Brisbane Corporate (Dept 003346)</t>
         </is>
       </c>
-      <c r="AH2" s="18" t="inlineStr">
+      <c r="AH2" s="17" t="inlineStr">
         <is>
           <t>Global</t>
         </is>
       </c>
-      <c r="AI2" s="18" t="inlineStr">
+      <c r="AI2" s="17" t="inlineStr">
         <is>
           <t>FORG</t>
         </is>
       </c>
-      <c r="AJ2" s="18" t="inlineStr">
+      <c r="AJ2" s="17" t="inlineStr">
         <is>
           <t>Unlisted Company, Foreign Public Company Registered with ASIC</t>
         </is>
       </c>
-      <c r="AK2" s="18" t="inlineStr">
+      <c r="AK2" s="17" t="inlineStr">
         <is>
           <t>&lt;This is randomly generated in the script&gt;</t>
         </is>
       </c>
-      <c r="AL2" s="18" t="inlineStr">
+      <c r="AL2" s="17" t="inlineStr">
         <is>
           <t>16-Feb-2017</t>
         </is>
       </c>
-      <c r="AM2" s="18" t="inlineStr">
+      <c r="AM2" s="17" t="inlineStr">
         <is>
           <t>Sydney, NSW,Australia</t>
         </is>
       </c>
-      <c r="AN2" s="18" t="inlineStr">
+      <c r="AN2" s="17" t="inlineStr">
         <is>
           <t>&lt;This is randomly generated in the script&gt;</t>
         </is>
       </c>
-      <c r="AO2" s="18" t="inlineStr">
+      <c r="AO2" s="17" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="AP2" s="18" t="inlineStr">
+      <c r="AP2" s="17" t="inlineStr">
         <is>
           <t>CBA</t>
         </is>
       </c>
-      <c r="AQ2" s="18" t="inlineStr">
+      <c r="AQ2" s="17" t="inlineStr">
         <is>
           <t>English</t>
         </is>
       </c>
-      <c r="AR2" s="18" t="inlineStr">
+      <c r="AR2" s="17" t="inlineStr">
         <is>
           <t>131100</t>
         </is>
       </c>
-      <c r="AS2" s="18" t="inlineStr">
+      <c r="AS2" s="17" t="inlineStr">
         <is>
           <t>SBLC, Loan</t>
         </is>
       </c>
-      <c r="AT2" s="18" t="inlineStr">
+      <c r="AT2" s="17" t="inlineStr">
         <is>
           <t>Principal, Interest, Fees</t>
         </is>
       </c>
-      <c r="AU2" s="18" t="inlineStr">
+      <c r="AU2" s="17" t="inlineStr">
         <is>
           <t>High Value Local RTGS (AUD)</t>
         </is>
       </c>
-      <c r="AV2" s="16" t="inlineStr">
+      <c r="AV2" s="15" t="inlineStr">
         <is>
           <t>RTGS1 - TO CUSTOMER</t>
         </is>
       </c>
-      <c r="AW2" s="16" t="inlineStr">
+      <c r="AW2" s="15" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AX2" s="17" t="inlineStr">
+      <c r="AX2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AY2" s="17" t="inlineStr">
+      <c r="AY2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AZ2" s="17" t="inlineStr">
+      <c r="AZ2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BA2" s="17" t="inlineStr">
+      <c r="BA2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BB2" s="17" t="inlineStr">
+      <c r="BB2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BC2" s="17" t="inlineStr">
+      <c r="BC2" s="16" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="BD2" s="17" t="inlineStr">
+      <c r="BD2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BE2" s="20" t="inlineStr">
+      <c r="BE2" s="19" t="inlineStr">
         <is>
           <t>Account Name: Anihant Trading Company
 Account Number: 066000 87654321</t>
         </is>
       </c>
-      <c r="BF2" s="17" t="inlineStr">
+      <c r="BF2" s="16" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="BG2" s="17" t="inlineStr">
+      <c r="BG2" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BH2" s="17" t="inlineStr">
+      <c r="BH2" s="16" t="inlineStr">
         <is>
           <t>MT103</t>
         </is>
       </c>
-      <c r="BI2" s="17" t="inlineStr">
+      <c r="BI2" s="16" t="inlineStr">
         <is>
           <t>Account With Institution</t>
         </is>
       </c>
-      <c r="BJ2" s="17" t="inlineStr">
+      <c r="BJ2" s="16" t="inlineStr">
         <is>
           <t>CTBAAU2S</t>
         </is>
       </c>
-      <c r="BK2" s="17" t="n"/>
-      <c r="BL2" s="17" t="n"/>
-      <c r="BM2" s="17" t="n"/>
-      <c r="BN2" s="17" t="n"/>
-      <c r="BO2" s="17" t="inlineStr">
+      <c r="BK2" s="16" t="n"/>
+      <c r="BL2" s="16" t="n"/>
+      <c r="BM2" s="16" t="n"/>
+      <c r="BN2" s="16" t="n"/>
+      <c r="BO2" s="16" t="inlineStr">
         <is>
           <t>Credit transfer - Service Level: None</t>
         </is>
       </c>
-      <c r="BP2" s="16" t="inlineStr">
+      <c r="BP2" s="15" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="BT2" s="16" t="inlineStr">
+      <c r="BT2" s="15" t="inlineStr">
         <is>
           <t>FJUSR01</t>
         </is>
       </c>
-      <c r="BU2" s="16" t="inlineStr">
+      <c r="BU2" s="15" t="inlineStr">
         <is>
           <t>password1</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="AV3" s="12" t="inlineStr">
+      <c r="AV3" s="11" t="inlineStr">
         <is>
           <t>RTGS1 - TO CUSTOMER</t>
         </is>
       </c>
-      <c r="BI3" s="12" t="inlineStr">
+      <c r="BI3" s="11" t="inlineStr">
         <is>
           <t>Beneficiary Customer</t>
         </is>
       </c>
-      <c r="BK3" s="12" t="inlineStr">
+      <c r="BK3" s="11" t="inlineStr">
         <is>
           <t>ARIHANT TRADING COMPANY</t>
         </is>
       </c>
-      <c r="BN3" s="12" t="inlineStr">
+      <c r="BN3" s="11" t="inlineStr">
         <is>
           <t>/06200087654321</t>
         </is>
       </c>
-      <c r="BT3" s="16" t="inlineStr">
+      <c r="BT3" s="15" t="inlineStr">
         <is>
           <t>FJAPR01</t>
         </is>
       </c>
-      <c r="BU3" s="16" t="inlineStr">
+      <c r="BU3" s="15" t="inlineStr">
         <is>
           <t>password2</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="AV4" s="12" t="inlineStr">
+      <c r="AV4" s="11" t="inlineStr">
         <is>
           <t>RTGS1 - TO CUSTOMER</t>
         </is>
       </c>
-      <c r="BI4" s="12" t="inlineStr">
+      <c r="BI4" s="11" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="BK4" s="12" t="inlineStr">
+      <c r="BK4" s="11" t="inlineStr">
         <is>
           <t>ARIHANT TRADING COMPANY</t>
         </is>
       </c>
-      <c r="BT4" s="16" t="inlineStr">
+      <c r="BT4" s="15" t="inlineStr">
         <is>
           <t>FJMGR01</t>
         </is>
       </c>
-      <c r="BU4" s="16" t="inlineStr">
+      <c r="BU4" s="15" t="inlineStr">
         <is>
           <t>password2</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="AU5" s="18" t="inlineStr">
+      <c r="AU5" s="17" t="inlineStr">
         <is>
           <t>High Value Local RTGS (AUD)</t>
         </is>
       </c>
-      <c r="AV5" s="16" t="inlineStr">
+      <c r="AV5" s="15" t="inlineStr">
         <is>
           <t>RTGS2 -FROM CUSTOMER</t>
         </is>
       </c>
-      <c r="AW5" s="16" t="inlineStr">
+      <c r="AW5" s="15" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="AX5" s="17" t="inlineStr">
+      <c r="AX5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AY5" s="17" t="inlineStr">
+      <c r="AY5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="AZ5" s="17" t="inlineStr">
+      <c r="AZ5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BA5" s="17" t="inlineStr">
+      <c r="BA5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BB5" s="17" t="inlineStr">
+      <c r="BB5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BC5" s="17" t="inlineStr">
+      <c r="BC5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BD5" s="17" t="inlineStr">
+      <c r="BD5" s="16" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="BE5" s="20" t="n"/>
-      <c r="BF5" s="17" t="inlineStr">
+      <c r="BE5" s="19" t="n"/>
+      <c r="BF5" s="16" t="inlineStr">
         <is>
           <t>OFF</t>
         </is>
       </c>
-      <c r="BG5" s="17" t="inlineStr">
+      <c r="BG5" s="16" t="inlineStr">
         <is>
           <t>ON</t>
         </is>
       </c>
-      <c r="BH5" s="17" t="inlineStr">
+      <c r="BH5" s="16" t="inlineStr">
         <is>
           <t>MT103</t>
         </is>
       </c>
-      <c r="BI5" s="17" t="inlineStr">
+      <c r="BI5" s="16" t="inlineStr">
         <is>
           <t>Account With Institution</t>
         </is>
       </c>
-      <c r="BJ5" s="17" t="inlineStr">
+      <c r="BJ5" s="16" t="inlineStr">
         <is>
           <t>CTBAAU2S</t>
         </is>
       </c>
-      <c r="BK5" s="17" t="n"/>
-      <c r="BL5" s="17" t="n"/>
-      <c r="BM5" s="17" t="n"/>
-      <c r="BN5" s="17" t="n"/>
-      <c r="BO5" s="17" t="inlineStr">
+      <c r="BK5" s="16" t="n"/>
+      <c r="BL5" s="16" t="n"/>
+      <c r="BM5" s="16" t="n"/>
+      <c r="BN5" s="16" t="n"/>
+      <c r="BO5" s="16" t="inlineStr">
         <is>
           <t>Credit transfer - Service Level: None</t>
         </is>
       </c>
-      <c r="BP5" s="16" t="inlineStr">
+      <c r="BP5" s="15" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="BQ5" s="16" t="n"/>
-      <c r="BR5" s="16" t="n"/>
-      <c r="BS5" s="16" t="n"/>
+      <c r="BQ5" s="15" t="n"/>
+      <c r="BR5" s="15" t="n"/>
+      <c r="BS5" s="15" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="AV6" s="16" t="inlineStr">
+      <c r="AV6" s="15" t="inlineStr">
         <is>
           <t>RTGS2 -FROM CUSTOMER</t>
         </is>
       </c>
-      <c r="BI6" s="12" t="inlineStr">
+      <c r="BI6" s="11" t="inlineStr">
         <is>
           <t>Beneficiary Customer</t>
         </is>
       </c>
-      <c r="BK6" s="12" t="inlineStr">
+      <c r="BK6" s="11" t="inlineStr">
         <is>
           <t>ARIHANT TRADING COMPANY</t>
         </is>
       </c>
-      <c r="BN6" s="12" t="inlineStr">
+      <c r="BN6" s="11" t="inlineStr">
         <is>
           <t>/06200087654321</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="11" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="AV7" s="16" t="inlineStr">
+      <c r="AV7" s="15" t="inlineStr">
         <is>
           <t>RTGS2 -FROM CUSTOMER</t>
         </is>
       </c>
-      <c r="BI7" s="12" t="inlineStr">
+      <c r="BI7" s="11" t="inlineStr">
         <is>
           <t>Ordering Customer</t>
         </is>
       </c>
-      <c r="BK7" s="12" t="inlineStr">
+      <c r="BK7" s="11" t="inlineStr">
         <is>
           <t>ARIHANT TRADING COMPANY</t>
         </is>
@@ -2110,7 +2148,7 @@
   <dimension ref="A1:BI3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2198,17 +2236,17 @@
           <t>Deal_AliasPrefix</t>
         </is>
       </c>
-      <c r="E1" s="15" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="F1" s="15" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Deal_Alias</t>
         </is>
       </c>
-      <c r="G1" s="15" t="inlineStr">
+      <c r="G1" s="14" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
@@ -2223,12 +2261,12 @@
           <t>Deal_SalesGroup</t>
         </is>
       </c>
-      <c r="J1" s="15" t="inlineStr">
+      <c r="J1" s="14" t="inlineStr">
         <is>
           <t>Borrower_ShortName</t>
         </is>
       </c>
-      <c r="K1" s="15" t="inlineStr">
+      <c r="K1" s="14" t="inlineStr">
         <is>
           <t>Borrower_Location</t>
         </is>
@@ -2463,7 +2501,7 @@
           <t>Primary_SGRIMethod</t>
         </is>
       </c>
-      <c r="BF1" s="15" t="inlineStr">
+      <c r="BF1" s="14" t="inlineStr">
         <is>
           <t>PrimaryFacility_Allocation</t>
         </is>
@@ -2507,17 +2545,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_14082020195230</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT414082020195230</t>
+          <t>UAT417082020131050</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -2532,7 +2570,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>1714417</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -2555,14 +2593,14 @@
           <t>Jones,  Vinnie</t>
         </is>
       </c>
-      <c r="O2" s="12" t="inlineStr">
+      <c r="O2" s="11" t="inlineStr">
         <is>
           <t>RTGS</t>
         </is>
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>%DBU</t>
+          <t>%OFAUSTCB001</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
@@ -2615,7 +2653,7 @@
           <t>25-May-2017</t>
         </is>
       </c>
-      <c r="AA2" s="21" t="inlineStr">
+      <c r="AA2" s="20" t="inlineStr">
         <is>
           <t>42,000,000.00</t>
         </is>
@@ -2795,7 +2833,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="BF3" s="1" t="inlineStr">
@@ -2819,8 +2857,8 @@
   </sheetPr>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2868,390 +2906,390 @@
     <col width="22.42578125" customWidth="1" style="1" min="41" max="41"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="22" thickBot="1">
-      <c r="A1" s="23" t="inlineStr">
+    <row r="1" ht="13.5" customFormat="1" customHeight="1" s="21" thickBot="1">
+      <c r="A1" s="22" t="inlineStr">
         <is>
           <t>rowid</t>
         </is>
       </c>
-      <c r="B1" s="23" t="inlineStr">
+      <c r="B1" s="22" t="inlineStr">
         <is>
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="24" t="inlineStr">
+      <c r="C1" s="23" t="inlineStr">
         <is>
           <t>Facility_NamePrefix</t>
         </is>
       </c>
-      <c r="D1" s="25" t="inlineStr">
+      <c r="D1" s="24" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="E1" s="25" t="inlineStr">
+      <c r="E1" s="24" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="F1" s="22" t="inlineStr">
+      <c r="F1" s="21" t="inlineStr">
         <is>
           <t>Deal_Currency</t>
         </is>
       </c>
-      <c r="G1" s="22" t="inlineStr">
+      <c r="G1" s="21" t="inlineStr">
         <is>
           <t>Facility_Type</t>
         </is>
       </c>
-      <c r="H1" s="22" t="inlineStr">
+      <c r="H1" s="21" t="inlineStr">
         <is>
           <t>Facility_ProposedCmtAmt</t>
         </is>
       </c>
-      <c r="I1" s="22" t="inlineStr">
+      <c r="I1" s="21" t="inlineStr">
         <is>
           <t>Facility_Currency</t>
         </is>
       </c>
-      <c r="J1" s="22" t="inlineStr">
+      <c r="J1" s="21" t="inlineStr">
         <is>
           <t>Facility_AgreementDate</t>
         </is>
       </c>
-      <c r="K1" s="22" t="inlineStr">
+      <c r="K1" s="21" t="inlineStr">
         <is>
           <t>Facility_EffectiveDate</t>
         </is>
       </c>
-      <c r="L1" s="22" t="inlineStr">
+      <c r="L1" s="21" t="inlineStr">
         <is>
           <t>Facility_ExpiryDate</t>
         </is>
       </c>
-      <c r="M1" s="22" t="inlineStr">
+      <c r="M1" s="21" t="inlineStr">
         <is>
           <t>Facility_MaturityDate</t>
         </is>
       </c>
-      <c r="N1" s="26" t="inlineStr">
+      <c r="N1" s="25" t="inlineStr">
         <is>
           <t>Facility_RiskType</t>
         </is>
       </c>
-      <c r="O1" s="26" t="inlineStr">
+      <c r="O1" s="25" t="inlineStr">
         <is>
           <t>Facility_LoanPurposeType</t>
         </is>
       </c>
-      <c r="P1" s="26" t="inlineStr">
+      <c r="P1" s="25" t="inlineStr">
         <is>
           <t>CurrencyLimit</t>
         </is>
       </c>
-      <c r="Q1" s="27" t="inlineStr">
+      <c r="Q1" s="26" t="inlineStr">
         <is>
           <t>Facility_Borrower</t>
         </is>
       </c>
-      <c r="R1" s="26" t="inlineStr">
+      <c r="R1" s="25" t="inlineStr">
         <is>
           <t>Borrower_Currency</t>
         </is>
       </c>
-      <c r="S1" s="26" t="inlineStr">
+      <c r="S1" s="25" t="inlineStr">
         <is>
           <t>Facility_BorrowerMaturity</t>
         </is>
       </c>
-      <c r="T1" s="26" t="inlineStr">
+      <c r="T1" s="25" t="inlineStr">
         <is>
           <t>Facility_BorrowerSGName</t>
         </is>
       </c>
-      <c r="U1" s="26" t="inlineStr">
+      <c r="U1" s="25" t="inlineStr">
         <is>
           <t>Facility_BorrowerPercent</t>
         </is>
       </c>
-      <c r="V1" s="26" t="inlineStr">
+      <c r="V1" s="25" t="inlineStr">
         <is>
           <t>Facility_GlobalLimit</t>
         </is>
       </c>
-      <c r="W1" s="26" t="inlineStr">
+      <c r="W1" s="25" t="inlineStr">
         <is>
           <t>FacilitySIC_Country</t>
         </is>
       </c>
-      <c r="X1" s="26" t="inlineStr">
+      <c r="X1" s="25" t="inlineStr">
         <is>
           <t>FacilitySIC_SearchBy</t>
         </is>
       </c>
-      <c r="Y1" s="26" t="inlineStr">
+      <c r="Y1" s="25" t="inlineStr">
         <is>
           <t>FacilitySIC_Code</t>
         </is>
       </c>
-      <c r="Z1" s="26" t="inlineStr">
+      <c r="Z1" s="25" t="inlineStr">
         <is>
           <t>FacilityMIS_Code</t>
         </is>
       </c>
-      <c r="AA1" s="26" t="inlineStr">
+      <c r="AA1" s="25" t="inlineStr">
         <is>
           <t>FacilityMIS_Value</t>
         </is>
       </c>
-      <c r="AB1" s="22" t="inlineStr">
+      <c r="AB1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_Category</t>
         </is>
       </c>
-      <c r="AC1" s="22" t="inlineStr">
+      <c r="AC1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_Type</t>
         </is>
       </c>
-      <c r="AD1" s="22" t="inlineStr">
+      <c r="AD1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_RateBasis</t>
         </is>
       </c>
-      <c r="AE1" s="22" t="inlineStr">
+      <c r="AE1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItem</t>
         </is>
       </c>
-      <c r="AF1" s="22" t="inlineStr">
+      <c r="AF1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_AfterItemType</t>
         </is>
       </c>
-      <c r="AG1" s="22" t="inlineStr">
+      <c r="AG1" s="21" t="inlineStr">
         <is>
           <t>FormulaCategory_Type</t>
         </is>
       </c>
-      <c r="AH1" s="22" t="inlineStr">
+      <c r="AH1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadType</t>
         </is>
       </c>
-      <c r="AI1" s="22" t="inlineStr">
+      <c r="AI1" s="21" t="inlineStr">
         <is>
           <t>OngoingFee_SpreadAmount</t>
         </is>
       </c>
-      <c r="AJ1" s="22" t="inlineStr">
+      <c r="AJ1" s="21" t="inlineStr">
         <is>
           <t>Interest_Category</t>
         </is>
       </c>
-      <c r="AK1" s="25" t="inlineStr">
+      <c r="AK1" s="24" t="inlineStr">
         <is>
           <t>Interest_OptionName</t>
         </is>
       </c>
-      <c r="AL1" s="22" t="inlineStr">
+      <c r="AL1" s="21" t="inlineStr">
         <is>
           <t>Interest_RateBasis</t>
         </is>
       </c>
-      <c r="AM1" s="22" t="inlineStr">
+      <c r="AM1" s="21" t="inlineStr">
         <is>
           <t>Interest_SpreadType</t>
         </is>
       </c>
-      <c r="AN1" s="22" t="inlineStr">
+      <c r="AN1" s="21" t="inlineStr">
         <is>
           <t>Interest_SpreadValue</t>
         </is>
       </c>
-      <c r="AO1" s="22" t="inlineStr">
+      <c r="AO1" s="21" t="inlineStr">
         <is>
           <t>Interest_BaseRateCode</t>
         </is>
       </c>
     </row>
-    <row r="2" customFormat="1" s="28">
-      <c r="A2" s="28" t="inlineStr">
+    <row r="2" customFormat="1" s="27">
+      <c r="A2" s="27" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="28" t="inlineStr">
+      <c r="B2" s="27" t="inlineStr">
         <is>
           <t>CBA_UAT_04</t>
         </is>
       </c>
-      <c r="C2" s="29" t="inlineStr">
+      <c r="C2" s="28" t="inlineStr">
         <is>
           <t>FAC-A_</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
-        </is>
-      </c>
-      <c r="F2" s="30" t="inlineStr">
+          <t>FAC-A_17082020131831</t>
+        </is>
+      </c>
+      <c r="F2" s="29" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="G2" s="29" t="inlineStr">
+      <c r="G2" s="28" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="H2" s="30" t="inlineStr">
+      <c r="H2" s="29" t="inlineStr">
         <is>
           <t>35,000,000.00</t>
         </is>
       </c>
-      <c r="I2" s="28" t="inlineStr">
+      <c r="I2" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J2" s="1" t="inlineStr">
-        <is>
-          <t>25-May-2017</t>
-        </is>
-      </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>07-Jun-2017</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>27-May-2019</t>
-        </is>
-      </c>
-      <c r="M2" s="1" t="inlineStr">
-        <is>
-          <t>27-May-2019</t>
-        </is>
-      </c>
-      <c r="N2" s="30" t="inlineStr">
+      <c r="J2" s="30" t="inlineStr">
+        <is>
+          <t>07-Jul-2020</t>
+        </is>
+      </c>
+      <c r="K2" s="30" t="inlineStr">
+        <is>
+          <t>07-Aug-2020</t>
+        </is>
+      </c>
+      <c r="L2" s="30" t="inlineStr">
+        <is>
+          <t>05-Aug-2022</t>
+        </is>
+      </c>
+      <c r="M2" s="30" t="inlineStr">
+        <is>
+          <t>05-Aug-2022</t>
+        </is>
+      </c>
+      <c r="N2" s="29" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="O2" s="28" t="inlineStr">
+      <c r="O2" s="27" t="inlineStr">
         <is>
           <t>Refinance of existing CBA/BW loan</t>
         </is>
       </c>
-      <c r="P2" s="28" t="inlineStr">
+      <c r="P2" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
-        </is>
-      </c>
-      <c r="R2" s="28" t="inlineStr">
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="R2" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="S2" s="28" t="inlineStr">
+      <c r="S2" s="27" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="T2" s="28" t="inlineStr">
+      <c r="T2" s="27" t="inlineStr">
         <is>
           <t>JONES</t>
         </is>
       </c>
-      <c r="U2" s="28" t="inlineStr">
+      <c r="U2" s="27" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="V2" s="28" t="inlineStr">
+      <c r="V2" s="27" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="W2" s="28" t="inlineStr">
+      <c r="W2" s="27" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="X2" s="28" t="inlineStr">
+      <c r="X2" s="27" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="Y2" s="28" t="inlineStr">
+      <c r="Y2" s="27" t="inlineStr">
         <is>
           <t>8710</t>
         </is>
       </c>
-      <c r="Z2" s="28" t="inlineStr">
+      <c r="Z2" s="27" t="inlineStr">
         <is>
           <t>RPLIM</t>
         </is>
       </c>
-      <c r="AA2" s="28" t="inlineStr">
+      <c r="AA2" s="27" t="inlineStr">
         <is>
           <t>RPL_Y</t>
         </is>
       </c>
-      <c r="AB2" s="28" t="inlineStr">
+      <c r="AB2" s="27" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="AC2" s="28" t="inlineStr">
+      <c r="AC2" s="27" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="AD2" s="28" t="inlineStr">
+      <c r="AD2" s="27" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AE2" s="28" t="inlineStr">
+      <c r="AE2" s="27" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="AF2" s="28" t="inlineStr">
+      <c r="AF2" s="27" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AG2" s="28" t="inlineStr">
+      <c r="AG2" s="27" t="inlineStr">
         <is>
           <t>Formula</t>
         </is>
       </c>
-      <c r="AH2" s="28" t="inlineStr">
+      <c r="AH2" s="27" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI2" s="28" t="inlineStr">
+      <c r="AI2" s="27" t="inlineStr">
         <is>
           <t>2.43</t>
         </is>
       </c>
-      <c r="AJ2" s="28" t="inlineStr">
+      <c r="AJ2" s="27" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
@@ -3261,204 +3299,204 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="AL2" s="28" t="inlineStr">
+      <c r="AL2" s="27" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AM2" s="28" t="inlineStr">
+      <c r="AM2" s="27" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AN2" s="28" t="inlineStr">
+      <c r="AN2" s="27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AO2" s="28" t="inlineStr">
+      <c r="AO2" s="27" t="inlineStr">
         <is>
           <t>BBSY</t>
         </is>
       </c>
     </row>
-    <row r="3" customFormat="1" s="28">
-      <c r="A3" s="28" t="inlineStr">
+    <row r="3" customFormat="1" s="27">
+      <c r="A3" s="27" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="28" t="inlineStr">
+      <c r="B3" s="27" t="inlineStr">
         <is>
           <t>CBA_UAT_04</t>
         </is>
       </c>
-      <c r="C3" s="29" t="inlineStr">
+      <c r="C3" s="28" t="inlineStr">
         <is>
           <t>FAC-B_</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
-        </is>
-      </c>
-      <c r="F3" s="30" t="inlineStr">
+          <t>FAC-B_17082020132715</t>
+        </is>
+      </c>
+      <c r="F3" s="29" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="G3" s="29" t="inlineStr">
+      <c r="G3" s="28" t="inlineStr">
         <is>
           <t>Term</t>
         </is>
       </c>
-      <c r="H3" s="30" t="inlineStr">
+      <c r="H3" s="29" t="inlineStr">
         <is>
           <t>7,000,000.00</t>
         </is>
       </c>
-      <c r="I3" s="28" t="inlineStr">
+      <c r="I3" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="J3" s="1" t="inlineStr">
-        <is>
-          <t>25-May-2017</t>
-        </is>
-      </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>07-Jun-2017</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>27-May-2019</t>
-        </is>
-      </c>
-      <c r="M3" s="1" t="inlineStr">
-        <is>
-          <t>27-May-2019</t>
-        </is>
-      </c>
-      <c r="N3" s="30" t="inlineStr">
+      <c r="J3" s="30" t="inlineStr">
+        <is>
+          <t>07-Jul-2020</t>
+        </is>
+      </c>
+      <c r="K3" s="30" t="inlineStr">
+        <is>
+          <t>07-Aug-2020</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>05-Aug-2022</t>
+        </is>
+      </c>
+      <c r="M3" s="30" t="inlineStr">
+        <is>
+          <t>05-Aug-2022</t>
+        </is>
+      </c>
+      <c r="N3" s="29" t="inlineStr">
         <is>
           <t>Loan</t>
         </is>
       </c>
-      <c r="O3" s="28" t="inlineStr">
+      <c r="O3" s="27" t="inlineStr">
         <is>
           <t>Refinance of existing CBA/BW loan</t>
         </is>
       </c>
-      <c r="P3" s="28" t="inlineStr">
+      <c r="P3" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
-        </is>
-      </c>
-      <c r="R3" s="28" t="inlineStr">
+          <t>BORROWER1111</t>
+        </is>
+      </c>
+      <c r="R3" s="27" t="inlineStr">
         <is>
           <t>AUD</t>
         </is>
       </c>
-      <c r="S3" s="28" t="inlineStr">
+      <c r="S3" s="27" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="T3" s="28" t="inlineStr">
+      <c r="T3" s="27" t="inlineStr">
         <is>
           <t>JONES</t>
         </is>
       </c>
-      <c r="U3" s="28" t="inlineStr">
+      <c r="U3" s="27" t="inlineStr">
         <is>
           <t>100.000000%</t>
         </is>
       </c>
-      <c r="V3" s="28" t="inlineStr">
+      <c r="V3" s="27" t="inlineStr">
         <is>
           <t>FLOAT</t>
         </is>
       </c>
-      <c r="W3" s="28" t="inlineStr">
+      <c r="W3" s="27" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="X3" s="28" t="inlineStr">
+      <c r="X3" s="27" t="inlineStr">
         <is>
           <t>Code</t>
         </is>
       </c>
-      <c r="Y3" s="28" t="inlineStr">
+      <c r="Y3" s="27" t="inlineStr">
         <is>
           <t>8710</t>
         </is>
       </c>
-      <c r="Z3" s="28" t="inlineStr">
+      <c r="Z3" s="27" t="inlineStr">
         <is>
           <t>RPLIM</t>
         </is>
       </c>
-      <c r="AA3" s="28" t="inlineStr">
+      <c r="AA3" s="27" t="inlineStr">
         <is>
           <t>RPL_Y</t>
         </is>
       </c>
-      <c r="AB3" s="28" t="inlineStr">
+      <c r="AB3" s="27" t="inlineStr">
         <is>
           <t>Facility Ongoing Fee</t>
         </is>
       </c>
-      <c r="AC3" s="28" t="inlineStr">
+      <c r="AC3" s="27" t="inlineStr">
         <is>
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="AD3" s="28" t="inlineStr">
+      <c r="AD3" s="27" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AE3" s="28" t="inlineStr">
+      <c r="AE3" s="27" t="inlineStr">
         <is>
           <t>FormulaCategory</t>
         </is>
       </c>
-      <c r="AF3" s="28" t="inlineStr">
+      <c r="AF3" s="27" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>
       </c>
-      <c r="AG3" s="28" t="inlineStr">
+      <c r="AG3" s="27" t="inlineStr">
         <is>
           <t>Formula</t>
         </is>
       </c>
-      <c r="AH3" s="28" t="inlineStr">
+      <c r="AH3" s="27" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AI3" s="28" t="inlineStr">
+      <c r="AI3" s="27" t="inlineStr">
         <is>
           <t>2.43</t>
         </is>
       </c>
-      <c r="AJ3" s="28" t="inlineStr">
+      <c r="AJ3" s="27" t="inlineStr">
         <is>
           <t>Option</t>
         </is>
@@ -3468,22 +3506,22 @@
           <t>BBSY - Bid</t>
         </is>
       </c>
-      <c r="AL3" s="28" t="inlineStr">
+      <c r="AL3" s="27" t="inlineStr">
         <is>
           <t>Actual/365</t>
         </is>
       </c>
-      <c r="AM3" s="28" t="inlineStr">
+      <c r="AM3" s="27" t="inlineStr">
         <is>
           <t>Percent</t>
         </is>
       </c>
-      <c r="AN3" s="28" t="inlineStr">
+      <c r="AN3" s="27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="AO3" s="28" t="inlineStr">
+      <c r="AO3" s="27" t="inlineStr">
         <is>
           <t>BBSY</t>
         </is>
@@ -3539,27 +3577,27 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="15" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="15" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="15" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="F1" s="15" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="G1" s="15" t="inlineStr">
+      <c r="G1" s="14" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
@@ -3599,19 +3637,19 @@
           <t>Loan_BorrowerBaseRate</t>
         </is>
       </c>
-      <c r="O1" s="15" t="inlineStr">
+      <c r="O1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="P1" s="15" t="inlineStr">
+      <c r="P1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3623,12 +3661,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -3638,7 +3676,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3656,7 +3694,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="J2" s="30" t="inlineStr">
+      <c r="J2" s="29" t="inlineStr">
         <is>
           <t>35,000,000.00</t>
         </is>
@@ -3693,7 +3731,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -3705,12 +3743,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -3720,7 +3758,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3738,7 +3776,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="J3" s="30" t="inlineStr">
+      <c r="J3" s="29" t="inlineStr">
         <is>
           <t>760,000.00</t>
         </is>
@@ -3775,7 +3813,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -3787,12 +3825,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -3802,7 +3840,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3820,7 +3858,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="J4" s="30" t="inlineStr">
+      <c r="J4" s="29" t="inlineStr">
         <is>
           <t>860,000.00</t>
         </is>
@@ -3857,7 +3895,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -3869,12 +3907,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -3884,7 +3922,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -3902,7 +3940,7 @@
           <t>AUD</t>
         </is>
       </c>
-      <c r="J5" s="30" t="inlineStr">
+      <c r="J5" s="29" t="inlineStr">
         <is>
           <t>500,000.00</t>
         </is>
@@ -3983,22 +4021,22 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="15" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="15" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="15" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="F1" s="15" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>OngoingFee_Alias</t>
         </is>
@@ -4023,19 +4061,19 @@
           <t>LineFeePayment_DueDate</t>
         </is>
       </c>
-      <c r="K1" s="15" t="inlineStr">
+      <c r="K1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="L1" s="15" t="inlineStr">
+      <c r="L1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4047,17 +4085,17 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -4092,7 +4130,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4104,17 +4142,17 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -4163,7 +4201,7 @@
   </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4203,32 +4241,32 @@
           <t>Test_Case</t>
         </is>
       </c>
-      <c r="C1" s="15" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>Deal_Name</t>
         </is>
       </c>
-      <c r="D1" s="15" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Facility_Name</t>
         </is>
       </c>
-      <c r="E1" s="15" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Loan_Alias</t>
         </is>
       </c>
-      <c r="F1" s="15" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>New_LoanAlias</t>
         </is>
       </c>
-      <c r="G1" s="15" t="inlineStr">
+      <c r="G1" s="14" t="inlineStr">
         <is>
           <t>Borrower_Name</t>
         </is>
       </c>
-      <c r="H1" s="15" t="inlineStr">
+      <c r="H1" s="14" t="inlineStr">
         <is>
           <t>Pricing_Option</t>
         </is>
@@ -4293,19 +4331,19 @@
           <t>FullRepayment_Reason</t>
         </is>
       </c>
-      <c r="U1" s="15" t="inlineStr">
+      <c r="U1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Description</t>
         </is>
       </c>
-      <c r="V1" s="15" t="inlineStr">
+      <c r="V1" s="14" t="inlineStr">
         <is>
           <t>Remittance_Instruction</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="12" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -4317,12 +4355,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4337,7 +4375,7 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -4377,7 +4415,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="12" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -4389,12 +4427,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -4409,7 +4447,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -4474,7 +4512,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="12" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>3</t>
         </is>
@@ -4486,12 +4524,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -4501,7 +4539,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -4566,7 +4604,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="12" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>4</t>
         </is>
@@ -4578,17 +4616,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_07102019143326</t>
+          <t>FAC-A_17082020131831</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -4653,7 +4691,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>5</t>
         </is>
@@ -4665,12 +4703,12 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -4685,7 +4723,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -4710,7 +4748,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="12" t="inlineStr">
+      <c r="A7" s="11" t="inlineStr">
         <is>
           <t>6</t>
         </is>
@@ -4722,12 +4760,12 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -4737,7 +4775,7 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -4762,7 +4800,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="12" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>7</t>
         </is>
@@ -4774,17 +4812,17 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -4809,7 +4847,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="12" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>8</t>
         </is>
@@ -4821,12 +4859,12 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
@@ -4841,7 +4879,7 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -4866,7 +4904,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12" t="inlineStr">
+      <c r="A10" s="11" t="inlineStr">
         <is>
           <t>9</t>
         </is>
@@ -4878,12 +4916,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -4893,7 +4931,7 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -4928,7 +4966,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="12" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>10</t>
         </is>
@@ -4940,17 +4978,17 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>UAT4_07102019143017</t>
+          <t>UAT4_17082020131050</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_07102019144013</t>
+          <t>FAC-B_17082020132715</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>1315059</t>
+          <t>BORROWER1111</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6729 update codes for EVG_CBAUAT04
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -878,7 +878,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 1714417</t>
+          <t>ARIHANT TRADING COMPANY 0915817</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
@@ -893,12 +893,12 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>1714417</t>
+          <t>0915817</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1714417</t>
+          <t>0915817</t>
         </is>
       </c>
       <c r="H2" s="5" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 1714417</t>
+          <t>ARIHANT TRADING COMPANY 0915817</t>
         </is>
       </c>
       <c r="D2" s="15" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>1714417</t>
+          <t>0915817</t>
         </is>
       </c>
       <c r="F2" s="16" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="O2" s="17" t="inlineStr">
         <is>
-          <t>1714417</t>
+          <t>0915817</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>1714417</t>
+          <t>0915817</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6731 Updated Files and Screenshots
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -516,9 +516,9 @@
   </sheetPr>
   <dimension ref="A1:CX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1131,8 +1131,8 @@
   </sheetPr>
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 1114706</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="D2" s="15" t="inlineStr">
@@ -1597,10 +1597,8 @@
           <t>Search by Customer ID</t>
         </is>
       </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>1114706</t>
-        </is>
+      <c r="E2" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="F2" s="16" t="inlineStr">
         <is>
@@ -1647,9 +1645,9 @@
           <t>Work Fax</t>
         </is>
       </c>
-      <c r="O2" s="17" t="inlineStr">
-        <is>
-          <t>1114706</t>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -1886,7 +1884,7 @@
       </c>
       <c r="BJ2" s="16" t="inlineStr">
         <is>
-          <t>CTBAAU2S</t>
+          <t>CTBAAU2SXXX</t>
         </is>
       </c>
       <c r="BK2" s="16" t="n"/>
@@ -2062,7 +2060,7 @@
       </c>
       <c r="BJ5" s="16" t="inlineStr">
         <is>
-          <t>CTBAAU2S</t>
+          <t>CTBAAU2SXXX</t>
         </is>
       </c>
       <c r="BK5" s="16" t="n"/>
@@ -2148,7 +2146,7 @@
   <dimension ref="A1:BI3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2201,17 +2199,17 @@
     <col width="16.140625" customWidth="1" style="1" min="47" max="47"/>
     <col width="34.140625" customWidth="1" style="1" min="48" max="48"/>
     <col width="28.85546875" customWidth="1" style="1" min="49" max="49"/>
-    <col width="31.28515625" customWidth="1" style="1" min="50" max="50"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="1" min="50" max="50"/>
     <col width="21" customWidth="1" style="1" min="51" max="51"/>
     <col width="26.140625" customWidth="1" style="1" min="52" max="52"/>
     <col width="24.5703125" customWidth="1" style="1" min="53" max="53"/>
     <col width="18.42578125" customWidth="1" style="1" min="54" max="54"/>
     <col width="21.140625" customWidth="1" style="1" min="55" max="55"/>
-    <col width="16.140625" customWidth="1" style="1" min="56" max="56"/>
+    <col width="28.140625" bestFit="1" customWidth="1" style="1" min="56" max="56"/>
     <col width="20.7109375" customWidth="1" style="1" min="57" max="57"/>
     <col width="25.28515625" customWidth="1" style="1" min="58" max="58"/>
     <col width="26.28515625" customWidth="1" style="1" min="59" max="59"/>
-    <col width="34.85546875" customWidth="1" style="1" min="60" max="60"/>
+    <col width="36.28515625" bestFit="1" customWidth="1" style="1" min="60" max="60"/>
     <col width="20" customWidth="1" style="1" min="61" max="61"/>
   </cols>
   <sheetData>
@@ -2545,17 +2543,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT417082020131050</t>
+          <t>UAT424082020185011</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -2570,7 +2568,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>1114706</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -2600,7 +2598,7 @@
       </c>
       <c r="P2" s="1" t="inlineStr">
         <is>
-          <t>%OFAUSTCB001</t>
+          <t>%AUSTCB001</t>
         </is>
       </c>
       <c r="Q2" s="1" t="inlineStr">
@@ -2770,7 +2768,7 @@
       </c>
       <c r="AX2" s="1" t="inlineStr">
         <is>
-          <t>COMMONWEALTH BANK AU-DBU</t>
+          <t>COMMONWEALTHBANKOFAUSTCB001</t>
         </is>
       </c>
       <c r="AY2" s="1" t="inlineStr">
@@ -2796,7 +2794,7 @@
       </c>
       <c r="BD2" s="1" t="inlineStr">
         <is>
-          <t>Lending,  Ops</t>
+          <t>AGENCY,  Lending and Leasing</t>
         </is>
       </c>
       <c r="BE2" s="1" t="inlineStr">
@@ -2833,7 +2831,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="BF3" s="1" t="inlineStr">
@@ -3131,12 +3129,12 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
@@ -3196,7 +3194,7 @@
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="R2" s="27" t="inlineStr">
@@ -3338,12 +3336,12 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="F3" s="29" t="inlineStr">
@@ -3403,7 +3401,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="R3" s="27" t="inlineStr">
@@ -3661,12 +3659,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -3676,7 +3674,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3743,12 +3741,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -3758,7 +3756,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3825,12 +3823,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -3840,7 +3838,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3907,12 +3905,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -3922,7 +3920,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -4085,22 +4083,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000004</t>
+          <t>ONG000000000313</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4142,22 +4140,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000005</t>
+          <t>ONG000000000314</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -4355,12 +4353,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4375,7 +4373,7 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -4427,12 +4425,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -4447,7 +4445,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -4524,12 +4522,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -4539,7 +4537,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -4616,17 +4614,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_17082020131831</t>
+          <t>FAC-A_24082020185912</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -4703,12 +4701,12 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -4723,7 +4721,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -4760,12 +4758,12 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -4775,7 +4773,7 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -4812,17 +4810,17 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -4859,12 +4857,12 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
@@ -4879,7 +4877,7 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -4916,12 +4914,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -4931,7 +4929,7 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -4978,17 +4976,17 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>UAT4_17082020131050</t>
+          <t>UAT4_24082020185011</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_17082020132715</t>
+          <t>FAC-B_24082020190924</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>BORROWER1111</t>
+          <t>ARIHANT TRADING COMPANY 000008</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6732 Update With New Codes Correct One Locator
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -1131,7 +1131,7 @@
   </sheetPr>
   <dimension ref="A1:BU7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3541,7 +3541,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000004</t>
+          <t>60000485</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -3697,14 +3697,14 @@
           <t>35,000,000.00</t>
         </is>
       </c>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>31-Oct-2018</t>
-        </is>
-      </c>
-      <c r="L2" s="1" t="inlineStr">
-        <is>
-          <t>30-Nov-2018</t>
+      <c r="K2" s="30" t="inlineStr">
+        <is>
+          <t>31-Oct-2020</t>
+        </is>
+      </c>
+      <c r="L2" s="30" t="inlineStr">
+        <is>
+          <t>30-Nov-2020</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>60000006</t>
+          <t>60000486</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -3779,14 +3779,14 @@
           <t>760,000.00</t>
         </is>
       </c>
-      <c r="K3" s="1" t="inlineStr">
-        <is>
-          <t>19-Nov-2018</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>19-Dec-2018</t>
+      <c r="K3" s="30" t="inlineStr">
+        <is>
+          <t>19-Nov-2020</t>
+        </is>
+      </c>
+      <c r="L3" s="30" t="inlineStr">
+        <is>
+          <t>19-Dec-2020</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000007</t>
+          <t>60000479</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
@@ -3861,14 +3861,14 @@
           <t>860,000.00</t>
         </is>
       </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>28-Nov-2018</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
-        <is>
-          <t>28-Dec-2018</t>
+      <c r="K4" s="30" t="inlineStr">
+        <is>
+          <t>28-Nov-2020</t>
+        </is>
+      </c>
+      <c r="L4" s="30" t="inlineStr">
+        <is>
+          <t>28-Dec-2020</t>
         </is>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -3943,14 +3943,14 @@
           <t>500,000.00</t>
         </is>
       </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>19-Feb-2019</t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>19-Mar-2019</t>
+      <c r="K5" s="30" t="inlineStr">
+        <is>
+          <t>19-Feb-2021</t>
+        </is>
+      </c>
+      <c r="L5" s="30" t="inlineStr">
+        <is>
+          <t>19-Mar-2021</t>
         </is>
       </c>
       <c r="M5" s="1" t="inlineStr">
@@ -3990,7 +3990,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4199,8 +4199,8 @@
   </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000004</t>
+          <t>60000485</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>60000006</t>
+          <t>60000486</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -4867,7 +4867,7 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>60000007</t>
+          <t>60000479</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6731 Update to takeout screenshot keywords in 04DealNotebook.robot
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -1589,7 +1589,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="D2" s="15" t="inlineStr">
@@ -1598,7 +1598,7 @@
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F2" s="16" t="inlineStr">
         <is>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="AJ2" s="17" t="inlineStr">
         <is>
-          <t>Unlisted Company, Foreign Public Company Registered with ASIC</t>
+          <t>Foreign Government, Foreign Government</t>
         </is>
       </c>
       <c r="AK2" s="17" t="inlineStr">
@@ -2543,17 +2543,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT424082020185011</t>
+          <t>UAT425082020161406</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="BF3" s="1" t="inlineStr">
@@ -3129,12 +3129,12 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="R2" s="27" t="inlineStr">
@@ -3336,12 +3336,12 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="F3" s="29" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="R3" s="27" t="inlineStr">
@@ -3659,12 +3659,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3741,12 +3741,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3823,12 +3823,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -3838,7 +3838,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3905,12 +3905,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -3920,7 +3920,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -4083,22 +4083,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000313</t>
+          <t>ONG000000000324</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4140,22 +4140,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000314</t>
+          <t>ONG000000000325</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -4353,12 +4353,12 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -4425,12 +4425,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -4445,7 +4445,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -4522,12 +4522,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -4537,7 +4537,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -4614,17 +4614,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_25082020162140</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -4701,12 +4701,12 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -4758,12 +4758,12 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -4810,17 +4810,17 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -4857,12 +4857,12 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
@@ -4877,7 +4877,7 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -4914,12 +4914,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -4976,17 +4976,17 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_25082020161406</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_25082020162950</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000010</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6732 Update 04Outstandings.robot EVG_CBAUAT04.xlsx and LIQ_LoanDrawdown_Locators.py
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -1132,7 +1132,7 @@
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2855,7 +2855,7 @@
   </sheetPr>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
@@ -3540,8 +3540,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3669,7 +3669,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000485</t>
+          <t>60000494</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -3704,7 +3704,7 @@
       </c>
       <c r="L2" s="30" t="inlineStr">
         <is>
-          <t>30-Nov-2020</t>
+          <t>11-Dec-2020</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>60000486</t>
+          <t>60000495</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000479</t>
+          <t>60000007</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
@@ -3990,7 +3990,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4199,8 +4199,8 @@
   </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000485</t>
+          <t>60000494</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>60000486</t>
+          <t>60000495</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -4867,7 +4867,7 @@
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>60000479</t>
+          <t>60000007</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6732 Update After Running Successfully { Create Outstandings for Deal D00000963 }
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UAT04_Runbook" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -150,7 +150,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -203,6 +203,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1132,7 +1136,7 @@
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1589,7 +1593,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="D2" s="15" t="inlineStr">
@@ -1598,7 +1602,7 @@
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="F2" s="16" t="inlineStr">
         <is>
@@ -1647,7 +1651,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -1720,7 +1724,7 @@
           <t>Australia</t>
         </is>
       </c>
-      <c r="AD2" s="17" t="inlineStr">
+      <c r="AD2" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">412345678
  </t>
@@ -1753,7 +1757,7 @@
       </c>
       <c r="AJ2" s="17" t="inlineStr">
         <is>
-          <t>Unlisted Company, Foreign Public Company Registered with ASIC</t>
+          <t>Foreign Government, Foreign Government</t>
         </is>
       </c>
       <c r="AK2" s="17" t="inlineStr">
@@ -2145,8 +2149,8 @@
   </sheetPr>
   <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2543,17 +2547,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT424082020185011</t>
+          <t>UAT427082020113709</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -2568,7 +2572,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -2636,19 +2640,19 @@
           <t>General Corp Purpose</t>
         </is>
       </c>
-      <c r="X2" s="1" t="inlineStr">
+      <c r="X2" s="33" t="inlineStr">
         <is>
           <t>25-May-2017</t>
         </is>
       </c>
-      <c r="Y2" s="1" t="inlineStr">
+      <c r="Y2" s="33" t="inlineStr">
         <is>
           <t>25-May-2017</t>
         </is>
       </c>
-      <c r="Z2" s="1" t="inlineStr">
-        <is>
-          <t>25-May-2017</t>
+      <c r="Z2" s="33" t="inlineStr">
+        <is>
+          <t>07-June-2017</t>
         </is>
       </c>
       <c r="AA2" s="20" t="inlineStr">
@@ -2831,7 +2835,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="BF3" s="1" t="inlineStr">
@@ -2855,8 +2859,8 @@
   </sheetPr>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3129,12 +3133,12 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
@@ -3159,22 +3163,22 @@
       </c>
       <c r="J2" s="30" t="inlineStr">
         <is>
-          <t>07-Jul-2020</t>
+          <t>25-May-2017</t>
         </is>
       </c>
       <c r="K2" s="30" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-Jun-2017</t>
         </is>
       </c>
       <c r="L2" s="30" t="inlineStr">
         <is>
-          <t>05-Aug-2022</t>
+          <t>27-May-2021</t>
         </is>
       </c>
       <c r="M2" s="30" t="inlineStr">
         <is>
-          <t>05-Aug-2022</t>
+          <t>27-May-2021</t>
         </is>
       </c>
       <c r="N2" s="29" t="inlineStr">
@@ -3194,7 +3198,7 @@
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="R2" s="27" t="inlineStr">
@@ -3336,12 +3340,12 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="F3" s="29" t="inlineStr">
@@ -3366,22 +3370,22 @@
       </c>
       <c r="J3" s="30" t="inlineStr">
         <is>
-          <t>07-Jul-2020</t>
+          <t>25-May-2017</t>
         </is>
       </c>
       <c r="K3" s="30" t="inlineStr">
         <is>
-          <t>07-Aug-2020</t>
+          <t>07-Jun-2017</t>
         </is>
       </c>
       <c r="L3" s="30" t="inlineStr">
         <is>
-          <t>05-Aug-2022</t>
+          <t>27-May-2021</t>
         </is>
       </c>
       <c r="M3" s="30" t="inlineStr">
         <is>
-          <t>05-Aug-2022</t>
+          <t>27-May-2021</t>
         </is>
       </c>
       <c r="N3" s="29" t="inlineStr">
@@ -3401,7 +3405,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="R3" s="27" t="inlineStr">
@@ -3540,8 +3544,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3659,22 +3663,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000494</t>
+          <t>60000560</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3697,14 +3701,14 @@
           <t>35,000,000.00</t>
         </is>
       </c>
-      <c r="K2" s="30" t="inlineStr">
-        <is>
-          <t>31-Oct-2020</t>
-        </is>
-      </c>
-      <c r="L2" s="30" t="inlineStr">
-        <is>
-          <t>11-Dec-2020</t>
+      <c r="K2" s="33" t="inlineStr">
+        <is>
+          <t>31-Oct-2018</t>
+        </is>
+      </c>
+      <c r="L2" s="33" t="inlineStr">
+        <is>
+          <t>30-Nov-2018</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr">
@@ -3741,22 +3745,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>60000495</t>
+          <t>60000561</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3779,14 +3783,14 @@
           <t>760,000.00</t>
         </is>
       </c>
-      <c r="K3" s="30" t="inlineStr">
-        <is>
-          <t>19-Nov-2020</t>
-        </is>
-      </c>
-      <c r="L3" s="30" t="inlineStr">
-        <is>
-          <t>19-Dec-2020</t>
+      <c r="K3" s="33" t="inlineStr">
+        <is>
+          <t>31-Oct-2018</t>
+        </is>
+      </c>
+      <c r="L3" s="33" t="inlineStr">
+        <is>
+          <t>30-Nov-2018</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr">
@@ -3823,22 +3827,22 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000007</t>
+          <t>60000562</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3861,14 +3865,14 @@
           <t>860,000.00</t>
         </is>
       </c>
-      <c r="K4" s="30" t="inlineStr">
-        <is>
-          <t>28-Nov-2020</t>
-        </is>
-      </c>
-      <c r="L4" s="30" t="inlineStr">
-        <is>
-          <t>28-Dec-2020</t>
+      <c r="K4" s="33" t="inlineStr">
+        <is>
+          <t>31-Oct-2018</t>
+        </is>
+      </c>
+      <c r="L4" s="33" t="inlineStr">
+        <is>
+          <t>30-Nov-2018</t>
         </is>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -3905,12 +3909,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -3920,7 +3924,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -3943,14 +3947,14 @@
           <t>500,000.00</t>
         </is>
       </c>
-      <c r="K5" s="30" t="inlineStr">
-        <is>
-          <t>19-Feb-2021</t>
-        </is>
-      </c>
-      <c r="L5" s="30" t="inlineStr">
-        <is>
-          <t>19-Mar-2021</t>
+      <c r="K5" s="33" t="inlineStr">
+        <is>
+          <t>31-Oct-2018</t>
+        </is>
+      </c>
+      <c r="L5" s="33" t="inlineStr">
+        <is>
+          <t>30-Nov-2018</t>
         </is>
       </c>
       <c r="M5" s="1" t="inlineStr">
@@ -4083,22 +4087,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000313</t>
+          <t>ONG000000000337</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4140,22 +4144,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000314</t>
+          <t>ONG000000000338</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -4353,17 +4357,17 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>60000494</t>
+          <t>60000560</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
@@ -4373,7 +4377,7 @@
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -4425,12 +4429,12 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -4445,7 +4449,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -4522,12 +4526,12 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -4537,7 +4541,7 @@
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -4614,17 +4618,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_24082020185912</t>
+          <t>FAC-A_27082020114456</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -4701,17 +4705,17 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>60000495</t>
+          <t>60000561</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
@@ -4721,7 +4725,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -4758,12 +4762,12 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -4773,7 +4777,7 @@
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -4810,17 +4814,17 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -4857,17 +4861,17 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>60000007</t>
+          <t>60000562</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
@@ -4877,7 +4881,7 @@
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -4914,12 +4918,12 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
@@ -4929,7 +4933,7 @@
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -4976,17 +4980,17 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>UAT4_24082020185011</t>
+          <t>UAT4_27082020113708</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_24082020190924</t>
+          <t>FAC-B_27082020115406</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000008</t>
+          <t>ARIHANT TRADING COMPANY 000015</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6858 Update 04Repricing.robot, EVG_CBAUAT04.xlsx, and LoanRepricing_Notebook.robot
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -32,7 +32,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
@@ -61,14 +61,14 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
       <color indexed="30"/>
       <sz val="10"/>
       <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
       <color theme="10"/>
       <sz val="10"/>
       <u val="single"/>
@@ -147,10 +147,10 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -207,6 +207,9 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1136,7 +1139,7 @@
   <dimension ref="A1:BU7"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -1155,7 +1158,7 @@
     <col width="22" customWidth="1" style="11" min="12" max="12"/>
     <col width="12.5703125" customWidth="1" style="11" min="13" max="13"/>
     <col width="15.7109375" customWidth="1" style="11" min="14" max="14"/>
-    <col width="23.7109375" customWidth="1" style="11" min="15" max="15"/>
+    <col width="34.85546875" bestFit="1" customWidth="1" style="11" min="15" max="15"/>
     <col width="18.28515625" customWidth="1" style="11" min="16" max="16"/>
     <col width="18.140625" customWidth="1" style="11" min="17" max="17"/>
     <col width="23.140625" customWidth="1" style="11" min="18" max="18"/>
@@ -1593,7 +1596,7 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="D2" s="15" t="inlineStr">
@@ -1602,7 +1605,7 @@
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="F2" s="16" t="inlineStr">
         <is>
@@ -1651,7 +1654,7 @@
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="P2" s="17" t="inlineStr">
@@ -1726,8 +1729,7 @@
       </c>
       <c r="AD2" s="34" t="inlineStr">
         <is>
-          <t xml:space="preserve">412345678
- </t>
+          <t>412345678</t>
         </is>
       </c>
       <c r="AE2" s="17" t="inlineStr">
@@ -2147,10 +2149,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BI14"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -2163,7 +2165,7 @@
     <col width="22" customWidth="1" style="1" min="7" max="7"/>
     <col width="14.42578125" customWidth="1" style="1" min="8" max="8"/>
     <col width="16.85546875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="20.85546875" customWidth="1" style="1" min="10" max="10"/>
+    <col width="34.85546875" bestFit="1" customWidth="1" style="1" min="10" max="10"/>
     <col width="22" customWidth="1" style="1" min="11" max="11"/>
     <col width="18.85546875" customWidth="1" style="1" min="12" max="12"/>
     <col width="19.7109375" customWidth="1" style="1" min="13" max="13"/>
@@ -2547,17 +2549,17 @@
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>UAT427082020113709</t>
+          <t>UAT410092020104911</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -2572,7 +2574,7 @@
       </c>
       <c r="J2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="K2" s="1" t="inlineStr">
@@ -2835,12 +2837,26 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="BF3" s="1" t="inlineStr">
         <is>
           <t>7,000,000.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="BA14" s="35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
+        </is>
+      </c>
+      <c r="BD14" s="35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+</t>
         </is>
       </c>
     </row>
@@ -2859,8 +2875,8 @@
   </sheetPr>
   <dimension ref="A1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3133,12 +3149,12 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="F2" s="29" t="inlineStr">
@@ -3173,12 +3189,12 @@
       </c>
       <c r="L2" s="30" t="inlineStr">
         <is>
-          <t>27-May-2021</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="M2" s="30" t="inlineStr">
         <is>
-          <t>27-May-2021</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="N2" s="29" t="inlineStr">
@@ -3198,7 +3214,7 @@
       </c>
       <c r="Q2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="R2" s="27" t="inlineStr">
@@ -3340,12 +3356,12 @@
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="F3" s="29" t="inlineStr">
@@ -3380,12 +3396,12 @@
       </c>
       <c r="L3" s="30" t="inlineStr">
         <is>
-          <t>27-May-2021</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="M3" s="30" t="inlineStr">
         <is>
-          <t>27-May-2021</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="N3" s="29" t="inlineStr">
@@ -3405,7 +3421,7 @@
       </c>
       <c r="Q3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="R3" s="27" t="inlineStr">
@@ -3544,8 +3560,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -3663,22 +3679,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>60000560</t>
+          <t>FAC-A_10092020105805</t>
+        </is>
+      </c>
+      <c r="E2" s="30" t="inlineStr">
+        <is>
+          <t>60000004</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -3708,7 +3724,7 @@
       </c>
       <c r="L2" s="33" t="inlineStr">
         <is>
-          <t>30-Nov-2018</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="M2" s="1" t="inlineStr">
@@ -3745,22 +3761,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>60000561</t>
+          <t>60000002</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -3785,12 +3801,12 @@
       </c>
       <c r="K3" s="33" t="inlineStr">
         <is>
-          <t>31-Oct-2018</t>
+          <t>19-Nov-2018</t>
         </is>
       </c>
       <c r="L3" s="33" t="inlineStr">
         <is>
-          <t>30-Nov-2018</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="M3" s="1" t="inlineStr">
@@ -3827,22 +3843,22 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000562</t>
+          <t>60000003</t>
         </is>
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -3867,12 +3883,12 @@
       </c>
       <c r="K4" s="33" t="inlineStr">
         <is>
-          <t>31-Oct-2018</t>
+          <t>28-Nov-2018</t>
         </is>
       </c>
       <c r="L4" s="33" t="inlineStr">
         <is>
-          <t>30-Nov-2018</t>
+          <t>27-May-2019</t>
         </is>
       </c>
       <c r="M4" s="1" t="inlineStr">
@@ -3909,12 +3925,12 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E5" s="1" t="inlineStr">
@@ -3924,7 +3940,7 @@
       </c>
       <c r="F5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
@@ -3949,12 +3965,12 @@
       </c>
       <c r="K5" s="33" t="inlineStr">
         <is>
-          <t>31-Oct-2018</t>
+          <t>19-Feb-2019</t>
         </is>
       </c>
       <c r="L5" s="33" t="inlineStr">
         <is>
-          <t>30-Nov-2018</t>
+          <t>19-Mar-2019</t>
         </is>
       </c>
       <c r="M5" s="1" t="inlineStr">
@@ -3993,8 +4009,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4087,22 +4103,22 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000337</t>
+          <t>ONG000000000002</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
@@ -4110,12 +4126,13 @@
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="I2" s="1" t="inlineStr">
-        <is>
-          <t>07-Dec-2018</t>
-        </is>
-      </c>
-      <c r="J2" s="1" t="inlineStr">
+      <c r="H2" s="11" t="n"/>
+      <c r="I2" s="30" t="inlineStr">
+        <is>
+          <t>07-Sep-2018</t>
+        </is>
+      </c>
+      <c r="J2" s="11" t="inlineStr">
         <is>
           <t>07-Dec-2018</t>
         </is>
@@ -4144,22 +4161,22 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>ONG000000000338</t>
+          <t>ONG000000000003</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
@@ -4167,12 +4184,13 @@
           <t>Line Fee</t>
         </is>
       </c>
-      <c r="I3" s="1" t="inlineStr">
-        <is>
-          <t>07-Dec-2018</t>
-        </is>
-      </c>
-      <c r="J3" s="1" t="inlineStr">
+      <c r="H3" s="11" t="n"/>
+      <c r="I3" s="30" t="inlineStr">
+        <is>
+          <t>07-Sep-2018</t>
+        </is>
+      </c>
+      <c r="J3" s="11" t="inlineStr">
         <is>
           <t>07-Dec-2018</t>
         </is>
@@ -4203,8 +4221,8 @@
   </sheetPr>
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4357,27 +4375,27 @@
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>60000560</t>
+          <t>FAC-A_10092020105805</t>
+        </is>
+      </c>
+      <c r="E2" s="30" t="inlineStr">
+        <is>
+          <t>60000004</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>60000026</t>
+          <t>60000007</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
@@ -4429,27 +4447,27 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
         <is>
-          <t>60000026</t>
+          <t>60000007</t>
         </is>
       </c>
       <c r="F3" s="1" t="inlineStr">
         <is>
-          <t>60000111</t>
+          <t>60000034</t>
         </is>
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -4526,22 +4544,22 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="E4" s="1" t="inlineStr">
         <is>
-          <t>60000111</t>
+          <t>60000034</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
@@ -4618,17 +4636,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
-          <t>FAC-A_27082020114456</t>
+          <t>FAC-A_10092020105805</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H5" s="1" t="inlineStr">
@@ -4705,27 +4723,27 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E6" s="1" t="inlineStr">
         <is>
-          <t>60000561</t>
+          <t>60000002</t>
         </is>
       </c>
       <c r="F6" s="1" t="inlineStr">
         <is>
-          <t>60000040</t>
+          <t>60000010</t>
         </is>
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -4762,22 +4780,22 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
         <is>
-          <t>60000040</t>
+          <t>60000010</t>
         </is>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
@@ -4814,17 +4832,17 @@
       </c>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
@@ -4861,27 +4879,27 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
-          <t>60000562</t>
+          <t>60000003</t>
         </is>
       </c>
       <c r="F9" s="1" t="inlineStr">
         <is>
-          <t>60000096</t>
+          <t>60000013</t>
         </is>
       </c>
       <c r="G9" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H9" s="1" t="inlineStr">
@@ -4918,22 +4936,22 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="E10" s="1" t="inlineStr">
         <is>
-          <t>60000096</t>
+          <t>60000013</t>
         </is>
       </c>
       <c r="G10" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -4980,17 +4998,17 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>UAT4_27082020113708</t>
+          <t>UAT4_10092020104911</t>
         </is>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
-          <t>FAC-B_27082020115406</t>
+          <t>FAC-B_10092020110713</t>
         </is>
       </c>
       <c r="G11" s="1" t="inlineStr">
         <is>
-          <t>ARIHANT TRADING COMPANY 000015</t>
+          <t>ARIHANT TRADING COMPANY 000021</t>
         </is>
       </c>
       <c r="H11" s="1" t="inlineStr">

</xml_diff>

<commit_message>
GDE-7025 Update Dataset 04
</commit_message>
<xml_diff>
--- a/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
+++ b/DataSet/CBAUATDeal_DataSet/EVG_CBAUAT04.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PTY001_QuickPartyOnboarding" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UAT04_Runbook" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -4222,7 +4222,7 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
@@ -4557,6 +4557,11 @@
           <t>60000034</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>60000041</t>
+        </is>
+      </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
           <t>ARIHANT TRADING COMPANY 000021</t>
@@ -4642,6 +4647,11 @@
       <c r="D5" s="1" t="inlineStr">
         <is>
           <t>FAC-A_10092020105805</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>60000041</t>
         </is>
       </c>
       <c r="G5" s="1" t="inlineStr">

</xml_diff>